<commit_message>
updated with a realistic Gantt Chart
</commit_message>
<xml_diff>
--- a/Rahman_SEG Application Project 2-Gantt Chart.xlsx
+++ b/Rahman_SEG Application Project 2-Gantt Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://teradynecom-my.sharepoint.com/personal/antara_rahman_teradyne_com/Documents/Desktop/New Hire/New Hire Tech/UFP New Hire Train/Project 2/SEG_UF-UFplus_Digital_Adv_FPGA_StudentPack_V2.2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://teradynecom-my.sharepoint.com/personal/antara_rahman_teradyne_com/Documents/Desktop/New Hire/New Hire Tech/UFP New Hire Train/Project 2/Project-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="374" documentId="8_{AF189AB5-A8E5-47FC-81D3-4BA9A6C17070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{570F980D-71D5-45E9-B816-4BFF894D86BC}"/>
+  <xr:revisionPtr revIDLastSave="443" documentId="8_{AF189AB5-A8E5-47FC-81D3-4BA9A6C17070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC9462A8-B10F-4653-852F-722ABE07AA56}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1110" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="0" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule1.0" sheetId="4" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>Test lists</t>
   </si>
   <si>
-    <t>Wrap Up - Schedule meeting with Mentor</t>
-  </si>
-  <si>
     <t>Wrap Up - SEP wrap up (ppt)</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>Final review meeting with Mentor</t>
+  </si>
+  <si>
+    <t>Wrap Up Presentation- Schedule meeting with Mentor</t>
   </si>
 </sst>
 </file>
@@ -301,7 +301,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +362,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="42">
     <border>
@@ -873,7 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -968,57 +974,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1030,22 +987,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1061,58 +1002,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1128,34 +1032,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1163,13 +1044,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1190,21 +1065,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1214,18 +1074,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1243,6 +1091,173 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1425,10 +1440,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1818,22 +1829,25 @@
   </sheetPr>
   <dimension ref="A1:AA124"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="121" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="120" customWidth="1"/>
+    <col min="2" max="2" width="20" style="78" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="77" customWidth="1"/>
     <col min="4" max="22" width="8" customWidth="1"/>
     <col min="24" max="24" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="100"/>
-      <c r="B1" s="100"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="23"/>
       <c r="D1" s="9" t="s">
         <v>0</v>
@@ -1860,11 +1874,11 @@
       <c r="X1" s="23"/>
     </row>
     <row r="2" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="101"/>
-      <c r="B2" s="68" t="s">
+      <c r="A2" s="65"/>
+      <c r="B2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="71" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="15"/>
@@ -1890,11 +1904,11 @@
       <c r="X2" s="24"/>
     </row>
     <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="101"/>
-      <c r="B3" s="68" t="s">
+      <c r="A3" s="65"/>
+      <c r="B3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="72" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="25"/>
@@ -1922,11 +1936,11 @@
       <c r="X3" s="24"/>
     </row>
     <row r="4" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="101"/>
-      <c r="B4" s="68" t="s">
+      <c r="A4" s="65"/>
+      <c r="B4" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="111" t="s">
+      <c r="C4" s="73" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="25"/>
@@ -1934,20 +1948,20 @@
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="G4" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="124"/>
+      <c r="O4" s="124"/>
+      <c r="P4" s="124"/>
+      <c r="Q4" s="124"/>
+      <c r="R4" s="124"/>
       <c r="S4" s="15"/>
       <c r="T4" s="15"/>
       <c r="U4" s="15"/>
@@ -1956,26 +1970,26 @@
       <c r="X4" s="24"/>
     </row>
     <row r="5" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="102"/>
-      <c r="B5" s="68" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="112"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="124"/>
+      <c r="M5" s="124"/>
+      <c r="N5" s="124"/>
+      <c r="O5" s="124"/>
+      <c r="P5" s="124"/>
+      <c r="Q5" s="124"/>
+      <c r="R5" s="124"/>
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
       <c r="U5" s="15"/>
@@ -1984,78 +1998,78 @@
       <c r="X5" s="24"/>
     </row>
     <row r="6" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="13"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="57" t="s">
+      <c r="C6" s="45"/>
+      <c r="D6" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="J6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="K6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="L6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="M6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="N6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="18" t="s">
+      <c r="O6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="P6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="Q6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="R6" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="19" t="s">
+      <c r="S6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="O6" s="19" t="s">
+      <c r="T6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="U6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="V6" s="20" t="s">
         <v>44</v>
-      </c>
-      <c r="R6" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="S6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" s="20" t="s">
-        <v>45</v>
       </c>
       <c r="W6" s="26"/>
       <c r="X6" s="27"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="58">
+      <c r="C7" s="51"/>
+      <c r="D7" s="44">
         <v>45551</v>
       </c>
       <c r="E7" s="28">
@@ -2136,14 +2150,14 @@
       <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="56">
+      <c r="A8" s="133">
         <v>1</v>
       </c>
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="125" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="103"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -2162,49 +2176,49 @@
       <c r="T8" s="20"/>
       <c r="U8" s="20"/>
       <c r="V8" s="20"/>
-      <c r="W8" s="66" t="s">
-        <v>23</v>
+      <c r="W8" s="48" t="s">
+        <v>22</v>
       </c>
       <c r="X8" s="32"/>
     </row>
     <row r="9" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="79"/>
-      <c r="N9" s="80"/>
-      <c r="O9" s="80"/>
-      <c r="P9" s="80"/>
-      <c r="Q9" s="80"/>
-      <c r="R9" s="80"/>
-      <c r="S9" s="81"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="81"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="64" t="s">
-        <v>25</v>
+      <c r="A9" s="87"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="128"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
+      <c r="V9" s="56"/>
+      <c r="W9" s="46" t="s">
+        <v>24</v>
       </c>
       <c r="X9" s="33"/>
       <c r="AA9" s="16"/>
     </row>
     <row r="10" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="56">
+      <c r="A10" s="133">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="103"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
@@ -2223,45 +2237,45 @@
       <c r="T10" s="20"/>
       <c r="U10" s="20"/>
       <c r="V10" s="20"/>
-      <c r="W10" s="64"/>
+      <c r="W10" s="46"/>
       <c r="X10" s="33"/>
     </row>
     <row r="11" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="79"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="80"/>
-      <c r="Q11" s="80"/>
-      <c r="R11" s="80"/>
-      <c r="S11" s="81"/>
-      <c r="T11" s="81"/>
-      <c r="U11" s="81"/>
-      <c r="V11" s="81"/>
-      <c r="W11" s="64"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="56"/>
+      <c r="V11" s="56"/>
+      <c r="W11" s="46"/>
       <c r="X11" s="33"/>
     </row>
     <row r="12" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="51">
+      <c r="A12" s="86">
         <f t="shared" ref="A12" si="2">A10+1</f>
         <v>3</v>
       </c>
-      <c r="B12" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="103"/>
+      <c r="B12" s="129" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="130"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -2280,46 +2294,46 @@
       <c r="T12" s="20"/>
       <c r="U12" s="20"/>
       <c r="V12" s="20"/>
-      <c r="W12" s="64"/>
+      <c r="W12" s="46"/>
       <c r="X12" s="33"/>
     </row>
     <row r="13" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="80"/>
-      <c r="P13" s="80"/>
-      <c r="Q13" s="80"/>
-      <c r="R13" s="80"/>
-      <c r="S13" s="81"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="81"/>
-      <c r="V13" s="81"/>
-      <c r="W13" s="64"/>
+      <c r="A13" s="87"/>
+      <c r="B13" s="131"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="56"/>
+      <c r="V13" s="56"/>
+      <c r="W13" s="46"/>
       <c r="X13" s="33"/>
     </row>
     <row r="14" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="51">
+      <c r="A14" s="86">
         <f t="shared" ref="A14" si="3">A12+1</f>
         <v>4</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="129" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="77"/>
+      <c r="C14" s="130"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="54"/>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -2337,45 +2351,45 @@
       <c r="T14" s="20"/>
       <c r="U14" s="20"/>
       <c r="V14" s="20"/>
-      <c r="W14" s="64"/>
+      <c r="W14" s="46"/>
       <c r="X14" s="33"/>
     </row>
     <row r="15" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-      <c r="K15" s="79"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="79"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="80"/>
-      <c r="P15" s="80"/>
-      <c r="Q15" s="80"/>
-      <c r="R15" s="80"/>
-      <c r="S15" s="81"/>
-      <c r="T15" s="81"/>
-      <c r="U15" s="81"/>
-      <c r="V15" s="81"/>
-      <c r="W15" s="64"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="131"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="55"/>
+      <c r="P15" s="55"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="46"/>
       <c r="X15" s="33"/>
     </row>
     <row r="16" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="51">
+      <c r="A16" s="86">
         <f t="shared" ref="A16:A20" si="4">A14+1</f>
         <v>5</v>
       </c>
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="129" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="57"/>
+      <c r="C16" s="130"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -2394,102 +2408,102 @@
       <c r="T16" s="20"/>
       <c r="U16" s="20"/>
       <c r="V16" s="20"/>
-      <c r="W16" s="64"/>
+      <c r="W16" s="46"/>
       <c r="X16" s="33"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="78"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="79"/>
-      <c r="K17" s="79"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="79"/>
-      <c r="N17" s="80"/>
-      <c r="O17" s="80"/>
-      <c r="P17" s="80"/>
-      <c r="Q17" s="80"/>
-      <c r="R17" s="80"/>
-      <c r="S17" s="81"/>
-      <c r="T17" s="81"/>
-      <c r="U17" s="81"/>
-      <c r="V17" s="81"/>
-      <c r="W17" s="64"/>
+      <c r="A17" s="87"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="132"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="55"/>
+      <c r="P17" s="55"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="46"/>
       <c r="X17" s="33"/>
     </row>
     <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="51">
+      <c r="A18" s="86">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="B18" s="129" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="130"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="124"/>
-      <c r="H18" s="124"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="95"/>
-      <c r="M18" s="95"/>
-      <c r="N18" s="125"/>
-      <c r="O18" s="125"/>
-      <c r="P18" s="125"/>
-      <c r="Q18" s="125"/>
-      <c r="R18" s="125"/>
-      <c r="S18" s="126"/>
-      <c r="T18" s="126"/>
-      <c r="U18" s="126"/>
-      <c r="V18" s="126"/>
-      <c r="W18" s="64"/>
+      <c r="B18" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="83"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="R18" s="59"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="46"/>
       <c r="X18" s="33"/>
     </row>
     <row r="19" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="131"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="124"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="124"/>
-      <c r="H19" s="124"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="125"/>
-      <c r="O19" s="125"/>
-      <c r="P19" s="125"/>
-      <c r="Q19" s="125"/>
-      <c r="R19" s="125"/>
-      <c r="S19" s="126"/>
-      <c r="T19" s="126"/>
-      <c r="U19" s="126"/>
-      <c r="V19" s="126"/>
-      <c r="W19" s="64"/>
+      <c r="A19" s="87"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="61"/>
+      <c r="T19" s="61"/>
+      <c r="U19" s="61"/>
+      <c r="V19" s="61"/>
+      <c r="W19" s="46"/>
       <c r="X19" s="33"/>
     </row>
     <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51">
+      <c r="A20" s="86">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="B20" s="129" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="130"/>
-      <c r="D20" s="57"/>
+      <c r="B20" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="83"/>
+      <c r="D20" s="43"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -2505,49 +2519,49 @@
       <c r="Q20" s="19"/>
       <c r="R20" s="19"/>
       <c r="S20" s="20"/>
-      <c r="T20" s="77"/>
+      <c r="T20" s="54"/>
       <c r="U20" s="20"/>
       <c r="V20" s="20"/>
-      <c r="W20" s="64"/>
+      <c r="W20" s="46"/>
       <c r="X20" s="33"/>
     </row>
     <row r="21" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="79"/>
-      <c r="K21" s="79"/>
-      <c r="L21" s="79"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="80"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="80"/>
-      <c r="R21" s="80"/>
-      <c r="S21" s="81"/>
-      <c r="T21" s="81"/>
-      <c r="U21" s="81"/>
-      <c r="V21" s="81"/>
-      <c r="W21" s="64"/>
+      <c r="A21" s="87"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+      <c r="V21" s="56"/>
+      <c r="W21" s="46"/>
       <c r="X21" s="33"/>
     </row>
     <row r="22" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="41">
+      <c r="A22" s="95">
         <f>A20+1</f>
         <v>8</v>
       </c>
-      <c r="B22" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="77"/>
+      <c r="B22" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="99"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="54"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
       <c r="H22" s="17"/>
@@ -2565,47 +2579,47 @@
       <c r="T22" s="20"/>
       <c r="U22" s="20"/>
       <c r="V22" s="20"/>
-      <c r="W22" s="64"/>
+      <c r="W22" s="46"/>
       <c r="X22" s="33"/>
     </row>
     <row r="23" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="79"/>
-      <c r="J23" s="79"/>
-      <c r="K23" s="79"/>
-      <c r="L23" s="79"/>
-      <c r="M23" s="79"/>
-      <c r="N23" s="80"/>
-      <c r="O23" s="80"/>
-      <c r="P23" s="80"/>
-      <c r="Q23" s="80"/>
-      <c r="R23" s="80"/>
-      <c r="S23" s="81"/>
-      <c r="T23" s="81"/>
-      <c r="U23" s="81"/>
-      <c r="V23" s="81"/>
-      <c r="W23" s="64"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="46"/>
       <c r="X23" s="33"/>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="41">
+      <c r="A24" s="95">
         <f>A22+1</f>
         <v>9</v>
       </c>
-      <c r="B24" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="17"/>
+      <c r="B24" s="98" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="99"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="54"/>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
       <c r="I24" s="18"/>
@@ -2622,48 +2636,48 @@
       <c r="T24" s="20"/>
       <c r="U24" s="20"/>
       <c r="V24" s="20"/>
-      <c r="W24" s="64"/>
+      <c r="W24" s="46"/>
       <c r="X24" s="33"/>
     </row>
     <row r="25" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="78"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="80"/>
-      <c r="O25" s="80"/>
-      <c r="P25" s="80"/>
-      <c r="Q25" s="80"/>
-      <c r="R25" s="80"/>
-      <c r="S25" s="81"/>
-      <c r="T25" s="81"/>
-      <c r="U25" s="81"/>
-      <c r="V25" s="81"/>
-      <c r="W25" s="64"/>
+      <c r="A25" s="95"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="56"/>
+      <c r="T25" s="56"/>
+      <c r="U25" s="56"/>
+      <c r="V25" s="56"/>
+      <c r="W25" s="46"/>
       <c r="X25" s="33"/>
     </row>
     <row r="26" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="41">
+      <c r="A26" s="95">
         <f>A24+1</f>
         <v>10</v>
       </c>
-      <c r="B26" s="60" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="57"/>
+      <c r="B26" s="98" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="99"/>
+      <c r="D26" s="43"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="17"/>
       <c r="I26" s="18"/>
       <c r="J26" s="18"/>
@@ -2679,49 +2693,49 @@
       <c r="T26" s="20"/>
       <c r="U26" s="20"/>
       <c r="V26" s="20"/>
-      <c r="W26" s="64"/>
+      <c r="W26" s="46"/>
       <c r="X26" s="33"/>
     </row>
     <row r="27" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="79"/>
-      <c r="J27" s="79"/>
-      <c r="K27" s="79"/>
-      <c r="L27" s="79"/>
-      <c r="M27" s="79"/>
-      <c r="N27" s="80"/>
-      <c r="O27" s="80"/>
-      <c r="P27" s="80"/>
-      <c r="Q27" s="80"/>
-      <c r="R27" s="80"/>
-      <c r="S27" s="81"/>
-      <c r="T27" s="81"/>
-      <c r="U27" s="81"/>
-      <c r="V27" s="81"/>
-      <c r="W27" s="64"/>
+      <c r="A27" s="95"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="52"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="52"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="52"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="56"/>
+      <c r="T27" s="56"/>
+      <c r="U27" s="56"/>
+      <c r="V27" s="56"/>
+      <c r="W27" s="46"/>
       <c r="X27" s="33"/>
     </row>
     <row r="28" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="41">
+      <c r="A28" s="95">
         <f>A26+1</f>
         <v>11</v>
       </c>
-      <c r="B28" s="60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="57"/>
+      <c r="B28" s="98" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="99"/>
+      <c r="D28" s="43"/>
       <c r="E28" s="17"/>
-      <c r="F28" s="77"/>
+      <c r="F28" s="43"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -2736,50 +2750,50 @@
       <c r="T28" s="20"/>
       <c r="U28" s="20"/>
       <c r="V28" s="20"/>
-      <c r="W28" s="64"/>
+      <c r="W28" s="46"/>
       <c r="X28" s="33"/>
     </row>
     <row r="29" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="78"/>
-      <c r="F29" s="78"/>
-      <c r="G29" s="78"/>
-      <c r="H29" s="78"/>
-      <c r="I29" s="79"/>
-      <c r="J29" s="79"/>
-      <c r="K29" s="79"/>
-      <c r="L29" s="79"/>
-      <c r="M29" s="79"/>
-      <c r="N29" s="80"/>
-      <c r="O29" s="80"/>
-      <c r="P29" s="80"/>
-      <c r="Q29" s="80"/>
-      <c r="R29" s="80"/>
-      <c r="S29" s="81"/>
-      <c r="T29" s="81"/>
-      <c r="U29" s="81"/>
-      <c r="V29" s="81"/>
-      <c r="W29" s="64"/>
+      <c r="A29" s="95"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="46"/>
       <c r="X29" s="33"/>
     </row>
     <row r="30" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41">
+      <c r="A30" s="95">
         <f>A28+1</f>
         <v>12</v>
       </c>
-      <c r="B30" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="61"/>
-      <c r="D30" s="57"/>
+      <c r="B30" s="98" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="99"/>
+      <c r="D30" s="43"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
-      <c r="G30" s="77"/>
+      <c r="G30" s="17"/>
       <c r="H30" s="17"/>
-      <c r="I30" s="18"/>
+      <c r="I30" s="62"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
@@ -2793,51 +2807,51 @@
       <c r="T30" s="20"/>
       <c r="U30" s="20"/>
       <c r="V30" s="20"/>
-      <c r="W30" s="64"/>
+      <c r="W30" s="46"/>
       <c r="X30" s="33"/>
     </row>
     <row r="31" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
-      <c r="M31" s="79"/>
-      <c r="N31" s="80"/>
-      <c r="O31" s="80"/>
-      <c r="P31" s="80"/>
-      <c r="Q31" s="80"/>
-      <c r="R31" s="80"/>
-      <c r="S31" s="81"/>
-      <c r="T31" s="81"/>
-      <c r="U31" s="81"/>
-      <c r="V31" s="81"/>
-      <c r="W31" s="64"/>
+      <c r="A31" s="95"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="55"/>
+      <c r="P31" s="55"/>
+      <c r="Q31" s="55"/>
+      <c r="R31" s="55"/>
+      <c r="S31" s="56"/>
+      <c r="T31" s="56"/>
+      <c r="U31" s="56"/>
+      <c r="V31" s="56"/>
+      <c r="W31" s="46"/>
       <c r="X31" s="33"/>
     </row>
     <row r="32" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="41">
+      <c r="A32" s="95">
         <f>A30+1</f>
         <v>13</v>
       </c>
-      <c r="B32" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="57"/>
+      <c r="B32" s="98" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="99"/>
+      <c r="D32" s="43"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
-      <c r="G32" s="77"/>
+      <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
+      <c r="J32" s="62"/>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
       <c r="M32" s="18"/>
@@ -2850,52 +2864,52 @@
       <c r="T32" s="20"/>
       <c r="U32" s="20"/>
       <c r="V32" s="20"/>
-      <c r="W32" s="64"/>
+      <c r="W32" s="46"/>
       <c r="X32" s="33"/>
     </row>
     <row r="33" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="41"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="79"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-      <c r="M33" s="79"/>
-      <c r="N33" s="80"/>
-      <c r="O33" s="80"/>
-      <c r="P33" s="80"/>
-      <c r="Q33" s="80"/>
-      <c r="R33" s="80"/>
-      <c r="S33" s="81"/>
-      <c r="T33" s="81"/>
-      <c r="U33" s="81"/>
-      <c r="V33" s="81"/>
-      <c r="W33" s="64"/>
+      <c r="A33" s="95"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="52"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="52"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="55"/>
+      <c r="P33" s="55"/>
+      <c r="Q33" s="55"/>
+      <c r="R33" s="55"/>
+      <c r="S33" s="56"/>
+      <c r="T33" s="56"/>
+      <c r="U33" s="56"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="46"/>
       <c r="X33" s="33"/>
     </row>
     <row r="34" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="41">
+      <c r="A34" s="95">
         <f>A32+1</f>
         <v>14</v>
       </c>
-      <c r="B34" s="60" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="57"/>
+      <c r="B34" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="99"/>
+      <c r="D34" s="43"/>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="77"/>
+      <c r="H34" s="17"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
+      <c r="K34" s="62"/>
       <c r="L34" s="18"/>
       <c r="M34" s="18"/>
       <c r="N34" s="19"/>
@@ -2907,53 +2921,53 @@
       <c r="T34" s="20"/>
       <c r="U34" s="20"/>
       <c r="V34" s="20"/>
-      <c r="W34" s="64"/>
+      <c r="W34" s="46"/>
       <c r="X34" s="33"/>
     </row>
     <row r="35" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="97"/>
-      <c r="E35" s="78"/>
-      <c r="F35" s="78"/>
-      <c r="G35" s="78"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="S35" s="81"/>
-      <c r="T35" s="81"/>
-      <c r="U35" s="81"/>
-      <c r="V35" s="81"/>
-      <c r="W35" s="64"/>
+      <c r="A35" s="95"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
+      <c r="P35" s="55"/>
+      <c r="Q35" s="55"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="56"/>
+      <c r="T35" s="56"/>
+      <c r="U35" s="56"/>
+      <c r="V35" s="56"/>
+      <c r="W35" s="46"/>
       <c r="X35" s="33"/>
     </row>
     <row r="36" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="41">
+      <c r="A36" s="95">
         <f>A34+1</f>
         <v>15</v>
       </c>
-      <c r="B36" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="61"/>
-      <c r="D36" s="57"/>
+      <c r="B36" s="98" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="99"/>
+      <c r="D36" s="43"/>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
-      <c r="H36" s="77"/>
+      <c r="H36" s="17"/>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
+      <c r="L36" s="62"/>
       <c r="M36" s="18"/>
       <c r="N36" s="19"/>
       <c r="O36" s="19"/>
@@ -2964,54 +2978,54 @@
       <c r="T36" s="20"/>
       <c r="U36" s="20"/>
       <c r="V36" s="20"/>
-      <c r="W36" s="64"/>
+      <c r="W36" s="46"/>
       <c r="X36" s="33"/>
     </row>
     <row r="37" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="61"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="80"/>
-      <c r="P37" s="80"/>
-      <c r="Q37" s="80"/>
-      <c r="R37" s="80"/>
-      <c r="S37" s="81"/>
-      <c r="T37" s="81"/>
-      <c r="U37" s="81"/>
-      <c r="V37" s="81"/>
-      <c r="W37" s="64"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="55"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="56"/>
+      <c r="T37" s="56"/>
+      <c r="U37" s="56"/>
+      <c r="V37" s="56"/>
+      <c r="W37" s="46"/>
       <c r="X37" s="33"/>
     </row>
     <row r="38" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="41">
+      <c r="A38" s="95">
         <f>A36+1</f>
         <v>16</v>
       </c>
-      <c r="B38" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="57"/>
+      <c r="B38" s="98" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="99"/>
+      <c r="D38" s="43"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
-      <c r="I38" s="77"/>
+      <c r="I38" s="18"/>
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
       <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
+      <c r="M38" s="62"/>
       <c r="N38" s="19"/>
       <c r="O38" s="19"/>
       <c r="P38" s="19"/>
@@ -3021,55 +3035,55 @@
       <c r="T38" s="20"/>
       <c r="U38" s="20"/>
       <c r="V38" s="20"/>
-      <c r="W38" s="64"/>
+      <c r="W38" s="46"/>
       <c r="X38" s="33"/>
     </row>
     <row r="39" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="41"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="78"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79"/>
-      <c r="N39" s="80"/>
-      <c r="O39" s="80"/>
-      <c r="P39" s="80"/>
-      <c r="Q39" s="80"/>
-      <c r="R39" s="80"/>
-      <c r="S39" s="81"/>
-      <c r="T39" s="81"/>
-      <c r="U39" s="81"/>
-      <c r="V39" s="81"/>
-      <c r="W39" s="64"/>
+      <c r="A39" s="95"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="53"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="52"/>
+      <c r="M39" s="58"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="55"/>
+      <c r="Q39" s="55"/>
+      <c r="R39" s="55"/>
+      <c r="S39" s="56"/>
+      <c r="T39" s="56"/>
+      <c r="U39" s="56"/>
+      <c r="V39" s="56"/>
+      <c r="W39" s="46"/>
       <c r="X39" s="33"/>
     </row>
     <row r="40" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="41">
+      <c r="A40" s="95">
         <f>A38+1</f>
         <v>17</v>
       </c>
-      <c r="B40" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="61"/>
-      <c r="D40" s="57"/>
+      <c r="B40" s="98" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="99"/>
+      <c r="D40" s="43"/>
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
       <c r="H40" s="17"/>
-      <c r="I40" s="77"/>
+      <c r="I40" s="18"/>
       <c r="J40" s="18"/>
       <c r="K40" s="18"/>
       <c r="L40" s="18"/>
       <c r="M40" s="18"/>
-      <c r="N40" s="19"/>
+      <c r="N40" s="134"/>
       <c r="O40" s="19"/>
       <c r="P40" s="19"/>
       <c r="Q40" s="19"/>
@@ -3078,56 +3092,56 @@
       <c r="T40" s="20"/>
       <c r="U40" s="20"/>
       <c r="V40" s="20"/>
-      <c r="W40" s="64"/>
+      <c r="W40" s="46"/>
       <c r="X40" s="33"/>
     </row>
     <row r="41" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="41"/>
-      <c r="B41" s="60"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="97"/>
-      <c r="E41" s="78"/>
-      <c r="F41" s="78"/>
-      <c r="G41" s="78"/>
-      <c r="H41" s="78"/>
-      <c r="I41" s="79"/>
-      <c r="J41" s="79"/>
-      <c r="K41" s="79"/>
-      <c r="L41" s="79"/>
-      <c r="M41" s="79"/>
-      <c r="N41" s="80"/>
-      <c r="O41" s="80"/>
-      <c r="P41" s="80"/>
-      <c r="Q41" s="80"/>
-      <c r="R41" s="80"/>
-      <c r="S41" s="81"/>
-      <c r="T41" s="81"/>
-      <c r="U41" s="81"/>
-      <c r="V41" s="81"/>
-      <c r="W41" s="64"/>
+      <c r="A41" s="95"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="99"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="53"/>
+      <c r="I41" s="52"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="55"/>
+      <c r="O41" s="55"/>
+      <c r="P41" s="55"/>
+      <c r="Q41" s="55"/>
+      <c r="R41" s="55"/>
+      <c r="S41" s="56"/>
+      <c r="T41" s="56"/>
+      <c r="U41" s="56"/>
+      <c r="V41" s="56"/>
+      <c r="W41" s="46"/>
       <c r="X41" s="33"/>
     </row>
     <row r="42" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="41">
+      <c r="A42" s="95">
         <f>A40+1</f>
         <v>18</v>
       </c>
-      <c r="B42" s="60" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="57"/>
+      <c r="B42" s="98" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="99"/>
+      <c r="D42" s="43"/>
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
       <c r="H42" s="17"/>
       <c r="I42" s="18"/>
-      <c r="J42" s="77"/>
+      <c r="J42" s="18"/>
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
       <c r="M42" s="18"/>
       <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
+      <c r="O42" s="134"/>
       <c r="P42" s="19"/>
       <c r="Q42" s="19"/>
       <c r="R42" s="19"/>
@@ -3135,218 +3149,218 @@
       <c r="T42" s="20"/>
       <c r="U42" s="20"/>
       <c r="V42" s="20"/>
-      <c r="W42" s="64"/>
+      <c r="W42" s="46"/>
       <c r="X42" s="33"/>
     </row>
     <row r="43" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="41"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="97"/>
-      <c r="E43" s="78"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="78"/>
-      <c r="H43" s="78"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="79"/>
-      <c r="N43" s="80"/>
-      <c r="O43" s="80"/>
-      <c r="P43" s="80"/>
-      <c r="Q43" s="80"/>
-      <c r="R43" s="80"/>
-      <c r="S43" s="81"/>
-      <c r="T43" s="81"/>
-      <c r="U43" s="81"/>
-      <c r="V43" s="81"/>
-      <c r="W43" s="64"/>
+      <c r="A43" s="95"/>
+      <c r="B43" s="98"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="55"/>
+      <c r="O43" s="55"/>
+      <c r="P43" s="55"/>
+      <c r="Q43" s="55"/>
+      <c r="R43" s="55"/>
+      <c r="S43" s="56"/>
+      <c r="T43" s="56"/>
+      <c r="U43" s="56"/>
+      <c r="V43" s="56"/>
+      <c r="W43" s="46"/>
       <c r="X43" s="33"/>
     </row>
     <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="41">
+      <c r="A44" s="95">
         <f>A42+1</f>
         <v>19</v>
       </c>
-      <c r="B44" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="57"/>
+      <c r="B44" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="99"/>
+      <c r="D44" s="43"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
       <c r="I44" s="18"/>
-      <c r="J44" s="77"/>
+      <c r="J44" s="18"/>
       <c r="K44" s="18"/>
       <c r="L44" s="18"/>
       <c r="M44" s="18"/>
       <c r="N44" s="19"/>
       <c r="O44" s="19"/>
-      <c r="P44" s="19"/>
+      <c r="P44" s="134"/>
       <c r="Q44" s="19"/>
       <c r="R44" s="19"/>
       <c r="S44" s="20"/>
       <c r="T44" s="20"/>
       <c r="U44" s="20"/>
       <c r="V44" s="20"/>
-      <c r="W44" s="64"/>
+      <c r="W44" s="46"/>
       <c r="X44" s="33"/>
     </row>
     <row r="45" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="41"/>
-      <c r="B45" s="60"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="97"/>
-      <c r="E45" s="78"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="78"/>
-      <c r="I45" s="79"/>
-      <c r="J45" s="79"/>
-      <c r="K45" s="79"/>
-      <c r="L45" s="79"/>
-      <c r="M45" s="79"/>
-      <c r="N45" s="80"/>
-      <c r="O45" s="80"/>
-      <c r="P45" s="80"/>
-      <c r="Q45" s="80"/>
-      <c r="R45" s="80"/>
-      <c r="S45" s="81"/>
-      <c r="T45" s="81"/>
-      <c r="U45" s="81"/>
-      <c r="V45" s="81"/>
-      <c r="W45" s="64"/>
+      <c r="A45" s="95"/>
+      <c r="B45" s="98"/>
+      <c r="C45" s="99"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="K45" s="52"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="55"/>
+      <c r="O45" s="55"/>
+      <c r="P45" s="55"/>
+      <c r="Q45" s="55"/>
+      <c r="R45" s="55"/>
+      <c r="S45" s="56"/>
+      <c r="T45" s="56"/>
+      <c r="U45" s="56"/>
+      <c r="V45" s="56"/>
+      <c r="W45" s="46"/>
       <c r="X45" s="33"/>
     </row>
     <row r="46" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="41">
+      <c r="A46" s="95">
         <f>A44+1</f>
         <v>20</v>
       </c>
-      <c r="B46" s="60" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="57"/>
+      <c r="B46" s="98" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="99"/>
+      <c r="D46" s="43"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
       <c r="H46" s="17"/>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
-      <c r="K46" s="77"/>
+      <c r="K46" s="18"/>
       <c r="L46" s="18"/>
       <c r="M46" s="18"/>
       <c r="N46" s="19"/>
       <c r="O46" s="19"/>
       <c r="P46" s="19"/>
-      <c r="Q46" s="19"/>
+      <c r="Q46" s="134"/>
       <c r="R46" s="19"/>
       <c r="S46" s="20"/>
       <c r="T46" s="20"/>
       <c r="U46" s="20"/>
       <c r="V46" s="20"/>
-      <c r="W46" s="64"/>
+      <c r="W46" s="46"/>
       <c r="X46" s="33"/>
     </row>
     <row r="47" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="41"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="97"/>
-      <c r="E47" s="78"/>
-      <c r="F47" s="78"/>
-      <c r="G47" s="78"/>
-      <c r="H47" s="78"/>
-      <c r="I47" s="79"/>
-      <c r="J47" s="79"/>
-      <c r="K47" s="79"/>
-      <c r="L47" s="79"/>
-      <c r="M47" s="79"/>
-      <c r="N47" s="80"/>
-      <c r="O47" s="80"/>
-      <c r="P47" s="80"/>
-      <c r="Q47" s="80"/>
-      <c r="R47" s="80"/>
-      <c r="S47" s="81"/>
-      <c r="T47" s="81"/>
-      <c r="U47" s="81"/>
-      <c r="V47" s="81"/>
-      <c r="W47" s="64"/>
+      <c r="A47" s="95"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="53"/>
+      <c r="H47" s="53"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="55"/>
+      <c r="O47" s="55"/>
+      <c r="P47" s="55"/>
+      <c r="Q47" s="55"/>
+      <c r="R47" s="55"/>
+      <c r="S47" s="56"/>
+      <c r="T47" s="56"/>
+      <c r="U47" s="56"/>
+      <c r="V47" s="56"/>
+      <c r="W47" s="46"/>
       <c r="X47" s="33"/>
     </row>
     <row r="48" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="41">
+      <c r="A48" s="95">
         <f>A46+1</f>
         <v>21</v>
       </c>
-      <c r="B48" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="57"/>
+      <c r="B48" s="98" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="99"/>
+      <c r="D48" s="43"/>
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
       <c r="I48" s="18"/>
       <c r="J48" s="18"/>
-      <c r="K48" s="77"/>
+      <c r="K48" s="18"/>
       <c r="L48" s="18"/>
       <c r="M48" s="18"/>
       <c r="N48" s="19"/>
       <c r="O48" s="19"/>
       <c r="P48" s="19"/>
       <c r="Q48" s="19"/>
-      <c r="R48" s="19"/>
+      <c r="R48" s="134"/>
       <c r="S48" s="20"/>
       <c r="T48" s="20"/>
       <c r="U48" s="20"/>
       <c r="V48" s="20"/>
-      <c r="W48" s="64"/>
+      <c r="W48" s="46"/>
       <c r="X48" s="33"/>
     </row>
     <row r="49" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="41"/>
-      <c r="B49" s="62"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="97"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
-      <c r="G49" s="78"/>
-      <c r="H49" s="78"/>
-      <c r="I49" s="79"/>
-      <c r="J49" s="79"/>
-      <c r="K49" s="79"/>
-      <c r="L49" s="79"/>
-      <c r="M49" s="79"/>
-      <c r="N49" s="80"/>
-      <c r="O49" s="80"/>
-      <c r="P49" s="80"/>
-      <c r="Q49" s="80"/>
-      <c r="R49" s="80"/>
-      <c r="S49" s="81"/>
-      <c r="T49" s="81"/>
-      <c r="U49" s="81"/>
-      <c r="V49" s="81"/>
-      <c r="W49" s="64"/>
+      <c r="A49" s="95"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="122"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="53"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="N49" s="55"/>
+      <c r="O49" s="55"/>
+      <c r="P49" s="55"/>
+      <c r="Q49" s="55"/>
+      <c r="R49" s="55"/>
+      <c r="S49" s="56"/>
+      <c r="T49" s="56"/>
+      <c r="U49" s="56"/>
+      <c r="V49" s="56"/>
+      <c r="W49" s="46"/>
       <c r="X49" s="33"/>
     </row>
     <row r="50" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="41">
+      <c r="A50" s="95">
         <f>A48+1</f>
         <v>22</v>
       </c>
-      <c r="B50" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="57"/>
+      <c r="B50" s="98" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="99"/>
+      <c r="D50" s="43"/>
       <c r="E50" s="17"/>
-      <c r="F50" s="77"/>
+      <c r="F50" s="54"/>
       <c r="G50" s="17"/>
       <c r="H50" s="17"/>
       <c r="I50" s="18"/>
@@ -3363,48 +3377,48 @@
       <c r="T50" s="20"/>
       <c r="U50" s="20"/>
       <c r="V50" s="20"/>
-      <c r="W50" s="64"/>
+      <c r="W50" s="46"/>
       <c r="X50" s="33"/>
     </row>
     <row r="51" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="41"/>
-      <c r="B51" s="60"/>
-      <c r="C51" s="61"/>
-      <c r="D51" s="97"/>
-      <c r="E51" s="78"/>
-      <c r="F51" s="78"/>
-      <c r="G51" s="78"/>
-      <c r="H51" s="78"/>
-      <c r="I51" s="79"/>
-      <c r="J51" s="79"/>
-      <c r="K51" s="79"/>
-      <c r="L51" s="79"/>
-      <c r="M51" s="79"/>
-      <c r="N51" s="80"/>
-      <c r="O51" s="80"/>
-      <c r="P51" s="80"/>
-      <c r="Q51" s="80"/>
-      <c r="R51" s="80"/>
-      <c r="S51" s="81"/>
-      <c r="T51" s="81"/>
-      <c r="U51" s="81"/>
-      <c r="V51" s="81"/>
-      <c r="W51" s="64"/>
+      <c r="A51" s="95"/>
+      <c r="B51" s="98"/>
+      <c r="C51" s="99"/>
+      <c r="D51" s="63"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="52"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="52"/>
+      <c r="N51" s="55"/>
+      <c r="O51" s="55"/>
+      <c r="P51" s="55"/>
+      <c r="Q51" s="55"/>
+      <c r="R51" s="55"/>
+      <c r="S51" s="56"/>
+      <c r="T51" s="56"/>
+      <c r="U51" s="56"/>
+      <c r="V51" s="56"/>
+      <c r="W51" s="46"/>
       <c r="X51" s="33"/>
     </row>
     <row r="52" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="41">
+      <c r="A52" s="95">
         <f>A50+1</f>
         <v>23</v>
       </c>
-      <c r="B52" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="57"/>
+      <c r="B52" s="98" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="99"/>
+      <c r="D52" s="43"/>
       <c r="E52" s="17"/>
-      <c r="F52" s="77"/>
-      <c r="G52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="54"/>
       <c r="H52" s="17"/>
       <c r="I52" s="18"/>
       <c r="J52" s="18"/>
@@ -3420,49 +3434,49 @@
       <c r="T52" s="20"/>
       <c r="U52" s="20"/>
       <c r="V52" s="20"/>
-      <c r="W52" s="64"/>
+      <c r="W52" s="46"/>
       <c r="X52" s="33"/>
     </row>
     <row r="53" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="41"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="97"/>
-      <c r="E53" s="78"/>
-      <c r="F53" s="78"/>
-      <c r="G53" s="78"/>
-      <c r="H53" s="78"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="79"/>
-      <c r="L53" s="79"/>
-      <c r="M53" s="79"/>
-      <c r="N53" s="80"/>
-      <c r="O53" s="80"/>
-      <c r="P53" s="80"/>
-      <c r="Q53" s="80"/>
-      <c r="R53" s="80"/>
-      <c r="S53" s="81"/>
-      <c r="T53" s="81"/>
-      <c r="U53" s="81"/>
-      <c r="V53" s="81"/>
-      <c r="W53" s="64"/>
+      <c r="A53" s="95"/>
+      <c r="B53" s="98"/>
+      <c r="C53" s="99"/>
+      <c r="D53" s="63"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="55"/>
+      <c r="O53" s="55"/>
+      <c r="P53" s="55"/>
+      <c r="Q53" s="55"/>
+      <c r="R53" s="55"/>
+      <c r="S53" s="56"/>
+      <c r="T53" s="56"/>
+      <c r="U53" s="56"/>
+      <c r="V53" s="56"/>
+      <c r="W53" s="46"/>
       <c r="X53" s="33"/>
     </row>
     <row r="54" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="41">
+      <c r="A54" s="95">
         <f>A52+1</f>
         <v>24</v>
       </c>
-      <c r="B54" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" s="61"/>
-      <c r="D54" s="57"/>
+      <c r="B54" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="99"/>
+      <c r="D54" s="43"/>
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
-      <c r="G54" s="77"/>
-      <c r="H54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="54"/>
       <c r="I54" s="18"/>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
@@ -3477,50 +3491,50 @@
       <c r="T54" s="20"/>
       <c r="U54" s="20"/>
       <c r="V54" s="20"/>
-      <c r="W54" s="64"/>
+      <c r="W54" s="46"/>
       <c r="X54" s="33"/>
     </row>
     <row r="55" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="41"/>
-      <c r="B55" s="60"/>
-      <c r="C55" s="61"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="78"/>
-      <c r="F55" s="78"/>
-      <c r="G55" s="78"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="79"/>
-      <c r="J55" s="79"/>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="79"/>
-      <c r="N55" s="80"/>
-      <c r="O55" s="80"/>
-      <c r="P55" s="80"/>
-      <c r="Q55" s="80"/>
-      <c r="R55" s="80"/>
-      <c r="S55" s="81"/>
-      <c r="T55" s="81"/>
-      <c r="U55" s="81"/>
-      <c r="V55" s="81"/>
-      <c r="W55" s="64"/>
+      <c r="A55" s="95"/>
+      <c r="B55" s="98"/>
+      <c r="C55" s="99"/>
+      <c r="D55" s="63"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="52"/>
+      <c r="J55" s="52"/>
+      <c r="K55" s="52"/>
+      <c r="L55" s="52"/>
+      <c r="M55" s="52"/>
+      <c r="N55" s="55"/>
+      <c r="O55" s="55"/>
+      <c r="P55" s="55"/>
+      <c r="Q55" s="55"/>
+      <c r="R55" s="55"/>
+      <c r="S55" s="56"/>
+      <c r="T55" s="56"/>
+      <c r="U55" s="56"/>
+      <c r="V55" s="56"/>
+      <c r="W55" s="46"/>
       <c r="X55" s="33"/>
     </row>
     <row r="56" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="41">
+      <c r="A56" s="95">
         <f>A54+1</f>
         <v>25</v>
       </c>
-      <c r="B56" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="57"/>
+      <c r="B56" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="99"/>
+      <c r="D56" s="43"/>
       <c r="E56" s="17"/>
       <c r="F56" s="17"/>
-      <c r="G56" s="77"/>
+      <c r="G56" s="17"/>
       <c r="H56" s="17"/>
-      <c r="I56" s="18"/>
+      <c r="I56" s="54"/>
       <c r="J56" s="18"/>
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
@@ -3534,51 +3548,51 @@
       <c r="T56" s="20"/>
       <c r="U56" s="20"/>
       <c r="V56" s="20"/>
-      <c r="W56" s="64"/>
+      <c r="W56" s="46"/>
       <c r="X56" s="33"/>
     </row>
     <row r="57" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="41"/>
-      <c r="B57" s="60"/>
-      <c r="C57" s="61"/>
-      <c r="D57" s="97"/>
-      <c r="E57" s="78"/>
-      <c r="F57" s="78"/>
-      <c r="G57" s="78"/>
-      <c r="H57" s="78"/>
-      <c r="I57" s="79"/>
-      <c r="J57" s="79"/>
-      <c r="K57" s="79"/>
-      <c r="L57" s="79"/>
-      <c r="M57" s="79"/>
-      <c r="N57" s="80"/>
-      <c r="O57" s="80"/>
-      <c r="P57" s="80"/>
-      <c r="Q57" s="80"/>
-      <c r="R57" s="80"/>
-      <c r="S57" s="81"/>
-      <c r="T57" s="81"/>
-      <c r="U57" s="81"/>
-      <c r="V57" s="81"/>
-      <c r="W57" s="64"/>
+      <c r="A57" s="95"/>
+      <c r="B57" s="98"/>
+      <c r="C57" s="99"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="53"/>
+      <c r="H57" s="53"/>
+      <c r="I57" s="52"/>
+      <c r="J57" s="52"/>
+      <c r="K57" s="52"/>
+      <c r="L57" s="52"/>
+      <c r="M57" s="52"/>
+      <c r="N57" s="55"/>
+      <c r="O57" s="55"/>
+      <c r="P57" s="55"/>
+      <c r="Q57" s="55"/>
+      <c r="R57" s="55"/>
+      <c r="S57" s="56"/>
+      <c r="T57" s="56"/>
+      <c r="U57" s="56"/>
+      <c r="V57" s="56"/>
+      <c r="W57" s="46"/>
       <c r="X57" s="33"/>
     </row>
     <row r="58" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="41">
+      <c r="A58" s="95">
         <f>A56+1</f>
         <v>26</v>
       </c>
-      <c r="B58" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="C58" s="61"/>
-      <c r="D58" s="57"/>
+      <c r="B58" s="98" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="99"/>
+      <c r="D58" s="43"/>
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
       <c r="G58" s="17"/>
-      <c r="H58" s="77"/>
+      <c r="H58" s="17"/>
       <c r="I58" s="18"/>
-      <c r="J58" s="18"/>
+      <c r="J58" s="54"/>
       <c r="K58" s="18"/>
       <c r="L58" s="18"/>
       <c r="M58" s="18"/>
@@ -3591,52 +3605,52 @@
       <c r="T58" s="20"/>
       <c r="U58" s="20"/>
       <c r="V58" s="20"/>
-      <c r="W58" s="64"/>
+      <c r="W58" s="46"/>
       <c r="X58" s="33"/>
     </row>
     <row r="59" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="41"/>
-      <c r="B59" s="60"/>
-      <c r="C59" s="61"/>
-      <c r="D59" s="97"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="78"/>
-      <c r="G59" s="78"/>
-      <c r="H59" s="78"/>
-      <c r="I59" s="79"/>
-      <c r="J59" s="79"/>
-      <c r="K59" s="79"/>
-      <c r="L59" s="79"/>
-      <c r="M59" s="79"/>
-      <c r="N59" s="80"/>
-      <c r="O59" s="80"/>
-      <c r="P59" s="80"/>
-      <c r="Q59" s="80"/>
-      <c r="R59" s="80"/>
-      <c r="S59" s="81"/>
-      <c r="T59" s="81"/>
-      <c r="U59" s="81"/>
-      <c r="V59" s="81"/>
-      <c r="W59" s="64"/>
+      <c r="A59" s="95"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="99"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="53"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="52"/>
+      <c r="J59" s="52"/>
+      <c r="K59" s="52"/>
+      <c r="L59" s="52"/>
+      <c r="M59" s="52"/>
+      <c r="N59" s="55"/>
+      <c r="O59" s="55"/>
+      <c r="P59" s="55"/>
+      <c r="Q59" s="55"/>
+      <c r="R59" s="55"/>
+      <c r="S59" s="56"/>
+      <c r="T59" s="56"/>
+      <c r="U59" s="56"/>
+      <c r="V59" s="56"/>
+      <c r="W59" s="46"/>
       <c r="X59" s="33"/>
     </row>
     <row r="60" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="41">
+      <c r="A60" s="95">
         <f>A58+1</f>
         <v>27</v>
       </c>
-      <c r="B60" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="57"/>
+      <c r="B60" s="98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" s="99"/>
+      <c r="D60" s="43"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
-      <c r="H60" s="77"/>
+      <c r="H60" s="17"/>
       <c r="I60" s="18"/>
       <c r="J60" s="18"/>
-      <c r="K60" s="18"/>
+      <c r="K60" s="54"/>
       <c r="L60" s="18"/>
       <c r="M60" s="18"/>
       <c r="N60" s="19"/>
@@ -3648,53 +3662,53 @@
       <c r="T60" s="20"/>
       <c r="U60" s="20"/>
       <c r="V60" s="20"/>
-      <c r="W60" s="64"/>
+      <c r="W60" s="46"/>
       <c r="X60" s="33"/>
     </row>
     <row r="61" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="78"/>
-      <c r="F61" s="78"/>
-      <c r="G61" s="78"/>
-      <c r="H61" s="78"/>
-      <c r="I61" s="79"/>
-      <c r="J61" s="79"/>
-      <c r="K61" s="79"/>
-      <c r="L61" s="79"/>
-      <c r="M61" s="79"/>
-      <c r="N61" s="80"/>
-      <c r="O61" s="80"/>
-      <c r="P61" s="80"/>
-      <c r="Q61" s="80"/>
-      <c r="R61" s="80"/>
-      <c r="S61" s="81"/>
-      <c r="T61" s="81"/>
-      <c r="U61" s="81"/>
-      <c r="V61" s="81"/>
-      <c r="W61" s="64"/>
+      <c r="A61" s="95"/>
+      <c r="B61" s="98"/>
+      <c r="C61" s="99"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="52"/>
+      <c r="J61" s="52"/>
+      <c r="K61" s="52"/>
+      <c r="L61" s="52"/>
+      <c r="M61" s="52"/>
+      <c r="N61" s="55"/>
+      <c r="O61" s="55"/>
+      <c r="P61" s="55"/>
+      <c r="Q61" s="55"/>
+      <c r="R61" s="55"/>
+      <c r="S61" s="56"/>
+      <c r="T61" s="56"/>
+      <c r="U61" s="56"/>
+      <c r="V61" s="56"/>
+      <c r="W61" s="46"/>
       <c r="X61" s="33"/>
     </row>
     <row r="62" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="41">
+      <c r="A62" s="95">
         <f>A60+1</f>
         <v>28</v>
       </c>
-      <c r="B62" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="57"/>
+      <c r="B62" s="98" t="s">
+        <v>51</v>
+      </c>
+      <c r="C62" s="99"/>
+      <c r="D62" s="43"/>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
       <c r="G62" s="17"/>
       <c r="H62" s="17"/>
-      <c r="I62" s="77"/>
+      <c r="I62" s="18"/>
       <c r="J62" s="18"/>
       <c r="K62" s="18"/>
-      <c r="L62" s="18"/>
+      <c r="L62" s="54"/>
       <c r="M62" s="18"/>
       <c r="N62" s="19"/>
       <c r="O62" s="19"/>
@@ -3705,54 +3719,54 @@
       <c r="T62" s="20"/>
       <c r="U62" s="20"/>
       <c r="V62" s="20"/>
-      <c r="W62" s="64"/>
+      <c r="W62" s="46"/>
       <c r="X62" s="33"/>
     </row>
     <row r="63" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="41"/>
-      <c r="B63" s="60"/>
-      <c r="C63" s="61"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="78"/>
-      <c r="F63" s="78"/>
-      <c r="G63" s="78"/>
-      <c r="H63" s="78"/>
-      <c r="I63" s="79"/>
-      <c r="J63" s="79"/>
-      <c r="K63" s="79"/>
-      <c r="L63" s="79"/>
-      <c r="M63" s="79"/>
-      <c r="N63" s="80"/>
-      <c r="O63" s="80"/>
-      <c r="P63" s="80"/>
-      <c r="Q63" s="80"/>
-      <c r="R63" s="80"/>
-      <c r="S63" s="81"/>
-      <c r="T63" s="81"/>
-      <c r="U63" s="81"/>
-      <c r="V63" s="81"/>
-      <c r="W63" s="64"/>
+      <c r="A63" s="95"/>
+      <c r="B63" s="98"/>
+      <c r="C63" s="99"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="52"/>
+      <c r="K63" s="52"/>
+      <c r="L63" s="52"/>
+      <c r="M63" s="52"/>
+      <c r="N63" s="55"/>
+      <c r="O63" s="55"/>
+      <c r="P63" s="55"/>
+      <c r="Q63" s="55"/>
+      <c r="R63" s="55"/>
+      <c r="S63" s="56"/>
+      <c r="T63" s="56"/>
+      <c r="U63" s="56"/>
+      <c r="V63" s="56"/>
+      <c r="W63" s="46"/>
       <c r="X63" s="33"/>
     </row>
     <row r="64" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="41">
+      <c r="A64" s="95">
         <f>A62+1</f>
         <v>29</v>
       </c>
-      <c r="B64" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="C64" s="61"/>
-      <c r="D64" s="57"/>
+      <c r="B64" s="98" t="s">
+        <v>52</v>
+      </c>
+      <c r="C64" s="99"/>
+      <c r="D64" s="43"/>
       <c r="E64" s="17"/>
       <c r="F64" s="17"/>
       <c r="G64" s="17"/>
       <c r="H64" s="17"/>
-      <c r="I64" s="77"/>
+      <c r="I64" s="18"/>
       <c r="J64" s="18"/>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
-      <c r="M64" s="18"/>
+      <c r="M64" s="54"/>
       <c r="N64" s="19"/>
       <c r="O64" s="19"/>
       <c r="P64" s="19"/>
@@ -3762,55 +3776,55 @@
       <c r="T64" s="20"/>
       <c r="U64" s="20"/>
       <c r="V64" s="20"/>
-      <c r="W64" s="64"/>
+      <c r="W64" s="46"/>
       <c r="X64" s="33"/>
     </row>
     <row r="65" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="41"/>
-      <c r="B65" s="60"/>
-      <c r="C65" s="61"/>
-      <c r="D65" s="97"/>
-      <c r="E65" s="78"/>
-      <c r="F65" s="78"/>
-      <c r="G65" s="78"/>
-      <c r="H65" s="78"/>
-      <c r="I65" s="79"/>
-      <c r="J65" s="79"/>
-      <c r="K65" s="79"/>
-      <c r="L65" s="79"/>
-      <c r="M65" s="79"/>
-      <c r="N65" s="80"/>
-      <c r="O65" s="80"/>
-      <c r="P65" s="80"/>
-      <c r="Q65" s="80"/>
-      <c r="R65" s="80"/>
-      <c r="S65" s="81"/>
-      <c r="T65" s="81"/>
-      <c r="U65" s="81"/>
-      <c r="V65" s="81"/>
-      <c r="W65" s="64"/>
+      <c r="A65" s="95"/>
+      <c r="B65" s="98"/>
+      <c r="C65" s="99"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
+      <c r="G65" s="53"/>
+      <c r="H65" s="53"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="52"/>
+      <c r="K65" s="52"/>
+      <c r="L65" s="52"/>
+      <c r="M65" s="52"/>
+      <c r="N65" s="55"/>
+      <c r="O65" s="55"/>
+      <c r="P65" s="55"/>
+      <c r="Q65" s="55"/>
+      <c r="R65" s="55"/>
+      <c r="S65" s="56"/>
+      <c r="T65" s="56"/>
+      <c r="U65" s="56"/>
+      <c r="V65" s="56"/>
+      <c r="W65" s="46"/>
       <c r="X65" s="33"/>
     </row>
     <row r="66" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="41">
+      <c r="A66" s="95">
         <f>A64+1</f>
         <v>30</v>
       </c>
-      <c r="B66" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="C66" s="61"/>
-      <c r="D66" s="57"/>
+      <c r="B66" s="98" t="s">
+        <v>53</v>
+      </c>
+      <c r="C66" s="99"/>
+      <c r="D66" s="43"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
       <c r="H66" s="17"/>
       <c r="I66" s="18"/>
-      <c r="J66" s="77"/>
+      <c r="J66" s="18"/>
       <c r="K66" s="18"/>
       <c r="L66" s="18"/>
       <c r="M66" s="18"/>
-      <c r="N66" s="19"/>
+      <c r="N66" s="134"/>
       <c r="O66" s="19"/>
       <c r="P66" s="19"/>
       <c r="Q66" s="19"/>
@@ -3819,239 +3833,239 @@
       <c r="T66" s="20"/>
       <c r="U66" s="20"/>
       <c r="V66" s="20"/>
-      <c r="W66" s="64"/>
+      <c r="W66" s="46"/>
       <c r="X66" s="33"/>
     </row>
     <row r="67" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="41"/>
-      <c r="B67" s="60"/>
-      <c r="C67" s="61"/>
-      <c r="D67" s="97"/>
-      <c r="E67" s="78"/>
-      <c r="F67" s="78"/>
-      <c r="G67" s="78"/>
-      <c r="H67" s="78"/>
-      <c r="I67" s="79"/>
-      <c r="J67" s="79"/>
-      <c r="K67" s="79"/>
-      <c r="L67" s="79"/>
-      <c r="M67" s="79"/>
-      <c r="N67" s="80"/>
-      <c r="O67" s="80"/>
-      <c r="P67" s="80"/>
-      <c r="Q67" s="80"/>
-      <c r="R67" s="80"/>
-      <c r="S67" s="81"/>
-      <c r="T67" s="81"/>
-      <c r="U67" s="81"/>
-      <c r="V67" s="81"/>
-      <c r="W67" s="64"/>
+      <c r="A67" s="95"/>
+      <c r="B67" s="98"/>
+      <c r="C67" s="99"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="53"/>
+      <c r="G67" s="53"/>
+      <c r="H67" s="53"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="52"/>
+      <c r="K67" s="52"/>
+      <c r="L67" s="52"/>
+      <c r="M67" s="52"/>
+      <c r="N67" s="55"/>
+      <c r="O67" s="55"/>
+      <c r="P67" s="55"/>
+      <c r="Q67" s="55"/>
+      <c r="R67" s="55"/>
+      <c r="S67" s="56"/>
+      <c r="T67" s="56"/>
+      <c r="U67" s="56"/>
+      <c r="V67" s="56"/>
+      <c r="W67" s="46"/>
       <c r="X67" s="33"/>
     </row>
     <row r="68" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="42">
+      <c r="A68" s="120">
         <v>31</v>
       </c>
-      <c r="B68" s="82" t="s">
+      <c r="B68" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="92"/>
+      <c r="D68" s="117"/>
+      <c r="E68" s="111"/>
+      <c r="F68" s="111"/>
+      <c r="G68" s="111"/>
+      <c r="H68" s="111"/>
+      <c r="I68" s="108"/>
+      <c r="J68" s="108"/>
+      <c r="K68" s="108"/>
+      <c r="L68" s="108"/>
+      <c r="M68" s="108"/>
+      <c r="N68" s="102"/>
+      <c r="O68" s="134"/>
+      <c r="P68" s="102"/>
+      <c r="Q68" s="102"/>
+      <c r="R68" s="102"/>
+      <c r="S68" s="105"/>
+      <c r="T68" s="105"/>
+      <c r="U68" s="105"/>
+      <c r="V68" s="105"/>
+      <c r="W68" s="46"/>
+      <c r="X68" s="33"/>
+    </row>
+    <row r="69" spans="1:24" ht="8.4499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="120"/>
+      <c r="B69" s="86"/>
+      <c r="C69" s="116"/>
+      <c r="D69" s="118"/>
+      <c r="E69" s="112"/>
+      <c r="F69" s="112"/>
+      <c r="G69" s="112"/>
+      <c r="H69" s="112"/>
+      <c r="I69" s="109"/>
+      <c r="J69" s="109"/>
+      <c r="K69" s="109"/>
+      <c r="L69" s="109"/>
+      <c r="M69" s="109"/>
+      <c r="N69" s="103"/>
+      <c r="O69" s="59"/>
+      <c r="P69" s="103"/>
+      <c r="Q69" s="103"/>
+      <c r="R69" s="103"/>
+      <c r="S69" s="106"/>
+      <c r="T69" s="106"/>
+      <c r="U69" s="106"/>
+      <c r="V69" s="106"/>
+      <c r="W69" s="46"/>
+      <c r="X69" s="33"/>
+    </row>
+    <row r="70" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="120"/>
+      <c r="B70" s="93"/>
+      <c r="C70" s="94"/>
+      <c r="D70" s="119"/>
+      <c r="E70" s="113"/>
+      <c r="F70" s="113"/>
+      <c r="G70" s="113"/>
+      <c r="H70" s="113"/>
+      <c r="I70" s="110"/>
+      <c r="J70" s="110"/>
+      <c r="K70" s="110"/>
+      <c r="L70" s="110"/>
+      <c r="M70" s="110"/>
+      <c r="N70" s="104"/>
+      <c r="O70" s="60"/>
+      <c r="P70" s="104"/>
+      <c r="Q70" s="104"/>
+      <c r="R70" s="104"/>
+      <c r="S70" s="107"/>
+      <c r="T70" s="107"/>
+      <c r="U70" s="107"/>
+      <c r="V70" s="107"/>
+      <c r="W70" s="46"/>
+      <c r="X70" s="33"/>
+    </row>
+    <row r="71" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="95">
+        <v>32</v>
+      </c>
+      <c r="B71" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="83"/>
-      <c r="D68" s="104"/>
-      <c r="E68" s="73"/>
-      <c r="F68" s="73"/>
-      <c r="G68" s="73"/>
-      <c r="H68" s="73"/>
-      <c r="I68" s="71"/>
-      <c r="J68" s="77"/>
-      <c r="K68" s="71"/>
-      <c r="L68" s="71"/>
-      <c r="M68" s="71"/>
-      <c r="N68" s="75"/>
-      <c r="O68" s="75"/>
-      <c r="P68" s="75"/>
-      <c r="Q68" s="75"/>
-      <c r="R68" s="75"/>
-      <c r="S68" s="76"/>
-      <c r="T68" s="76"/>
-      <c r="U68" s="76"/>
-      <c r="V68" s="76"/>
-      <c r="W68" s="64"/>
-      <c r="X68" s="33"/>
-    </row>
-    <row r="69" spans="1:24" ht="8.4499999999999993" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="42"/>
-      <c r="B69" s="51"/>
-      <c r="C69" s="52"/>
-      <c r="D69" s="105"/>
-      <c r="E69" s="86"/>
-      <c r="F69" s="86"/>
-      <c r="G69" s="86"/>
-      <c r="H69" s="86"/>
-      <c r="I69" s="87"/>
-      <c r="J69" s="79"/>
-      <c r="K69" s="87"/>
-      <c r="L69" s="87"/>
-      <c r="M69" s="87"/>
-      <c r="N69" s="88"/>
-      <c r="O69" s="88"/>
-      <c r="P69" s="88"/>
-      <c r="Q69" s="88"/>
-      <c r="R69" s="88"/>
-      <c r="S69" s="90"/>
-      <c r="T69" s="90"/>
-      <c r="U69" s="90"/>
-      <c r="V69" s="90"/>
-      <c r="W69" s="64"/>
-      <c r="X69" s="33"/>
-    </row>
-    <row r="70" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="42"/>
-      <c r="B70" s="84"/>
-      <c r="C70" s="85"/>
-      <c r="D70" s="106"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
-      <c r="I70" s="72"/>
-      <c r="J70" s="79"/>
-      <c r="K70" s="72"/>
-      <c r="L70" s="72"/>
-      <c r="M70" s="72"/>
-      <c r="N70" s="89"/>
-      <c r="O70" s="89"/>
-      <c r="P70" s="89"/>
-      <c r="Q70" s="89"/>
-      <c r="R70" s="89"/>
-      <c r="S70" s="91"/>
-      <c r="T70" s="91"/>
-      <c r="U70" s="91"/>
-      <c r="V70" s="91"/>
-      <c r="W70" s="64"/>
-      <c r="X70" s="33"/>
-    </row>
-    <row r="71" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="41">
-        <v>32</v>
-      </c>
-      <c r="B71" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" s="61"/>
-      <c r="D71" s="57"/>
+      <c r="C71" s="99"/>
+      <c r="D71" s="43"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
       <c r="G71" s="17"/>
       <c r="H71" s="17"/>
       <c r="I71" s="18"/>
       <c r="J71" s="18"/>
-      <c r="K71" s="77"/>
+      <c r="K71" s="18"/>
       <c r="L71" s="18"/>
       <c r="M71" s="18"/>
       <c r="N71" s="19"/>
       <c r="O71" s="19"/>
-      <c r="P71" s="19"/>
+      <c r="P71" s="134"/>
       <c r="Q71" s="19"/>
       <c r="R71" s="19"/>
       <c r="S71" s="20"/>
       <c r="T71" s="20"/>
       <c r="U71" s="20"/>
       <c r="V71" s="20"/>
-      <c r="W71" s="64"/>
+      <c r="W71" s="46"/>
       <c r="X71" s="33"/>
     </row>
     <row r="72" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="41"/>
-      <c r="B72" s="60"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="97"/>
-      <c r="E72" s="78"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="78"/>
-      <c r="H72" s="78"/>
-      <c r="I72" s="79"/>
-      <c r="J72" s="79"/>
-      <c r="K72" s="79"/>
-      <c r="L72" s="79"/>
-      <c r="M72" s="79"/>
-      <c r="N72" s="80"/>
-      <c r="O72" s="80"/>
-      <c r="P72" s="80"/>
-      <c r="Q72" s="80"/>
-      <c r="R72" s="80"/>
-      <c r="S72" s="81"/>
-      <c r="T72" s="81"/>
-      <c r="U72" s="81"/>
-      <c r="V72" s="81"/>
-      <c r="W72" s="64"/>
+      <c r="A72" s="95"/>
+      <c r="B72" s="98"/>
+      <c r="C72" s="99"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
+      <c r="H72" s="53"/>
+      <c r="I72" s="52"/>
+      <c r="J72" s="52"/>
+      <c r="K72" s="52"/>
+      <c r="L72" s="52"/>
+      <c r="M72" s="52"/>
+      <c r="N72" s="55"/>
+      <c r="O72" s="55"/>
+      <c r="P72" s="55"/>
+      <c r="Q72" s="55"/>
+      <c r="R72" s="55"/>
+      <c r="S72" s="56"/>
+      <c r="T72" s="56"/>
+      <c r="U72" s="56"/>
+      <c r="V72" s="56"/>
+      <c r="W72" s="46"/>
       <c r="X72" s="33"/>
     </row>
     <row r="73" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="51">
+      <c r="A73" s="86">
         <v>33</v>
       </c>
-      <c r="B73" s="60" t="s">
-        <v>62</v>
-      </c>
-      <c r="C73" s="61"/>
-      <c r="D73" s="57"/>
+      <c r="B73" s="98" t="s">
+        <v>61</v>
+      </c>
+      <c r="C73" s="99"/>
+      <c r="D73" s="43"/>
       <c r="E73" s="17"/>
       <c r="F73" s="17"/>
       <c r="G73" s="17"/>
       <c r="H73" s="17"/>
       <c r="I73" s="18"/>
       <c r="J73" s="18"/>
-      <c r="K73" s="77"/>
+      <c r="K73" s="18"/>
       <c r="L73" s="18"/>
       <c r="M73" s="18"/>
       <c r="N73" s="19"/>
       <c r="O73" s="19"/>
       <c r="P73" s="19"/>
-      <c r="Q73" s="19"/>
+      <c r="Q73" s="134"/>
       <c r="R73" s="19"/>
       <c r="S73" s="20"/>
       <c r="T73" s="20"/>
       <c r="U73" s="20"/>
       <c r="V73" s="20"/>
-      <c r="W73" s="64"/>
+      <c r="W73" s="46"/>
       <c r="X73" s="33"/>
     </row>
     <row r="74" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="53"/>
-      <c r="B74" s="60"/>
-      <c r="C74" s="61"/>
-      <c r="D74" s="97"/>
-      <c r="E74" s="78"/>
-      <c r="F74" s="78"/>
-      <c r="G74" s="78"/>
-      <c r="H74" s="78"/>
-      <c r="I74" s="79"/>
-      <c r="J74" s="79"/>
-      <c r="K74" s="79"/>
-      <c r="L74" s="79"/>
-      <c r="M74" s="79"/>
-      <c r="N74" s="80"/>
-      <c r="O74" s="80"/>
-      <c r="P74" s="80"/>
-      <c r="Q74" s="80"/>
-      <c r="R74" s="80"/>
-      <c r="S74" s="81"/>
-      <c r="T74" s="81"/>
-      <c r="U74" s="81"/>
-      <c r="V74" s="81"/>
-      <c r="W74" s="64"/>
+      <c r="A74" s="87"/>
+      <c r="B74" s="98"/>
+      <c r="C74" s="99"/>
+      <c r="D74" s="63"/>
+      <c r="E74" s="53"/>
+      <c r="F74" s="53"/>
+      <c r="G74" s="53"/>
+      <c r="H74" s="53"/>
+      <c r="I74" s="52"/>
+      <c r="J74" s="52"/>
+      <c r="K74" s="52"/>
+      <c r="L74" s="52"/>
+      <c r="M74" s="52"/>
+      <c r="N74" s="55"/>
+      <c r="O74" s="55"/>
+      <c r="P74" s="55"/>
+      <c r="Q74" s="55"/>
+      <c r="R74" s="55"/>
+      <c r="S74" s="56"/>
+      <c r="T74" s="56"/>
+      <c r="U74" s="56"/>
+      <c r="V74" s="56"/>
+      <c r="W74" s="46"/>
       <c r="X74" s="33"/>
     </row>
     <row r="75" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="51">
+      <c r="A75" s="86">
         <f t="shared" ref="A75" si="5">A73+1</f>
         <v>34</v>
       </c>
-      <c r="B75" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C75" s="61"/>
-      <c r="D75" s="57"/>
+      <c r="B75" s="98" t="s">
+        <v>62</v>
+      </c>
+      <c r="C75" s="99"/>
+      <c r="D75" s="43"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17"/>
       <c r="G75" s="17"/>
@@ -4059,56 +4073,56 @@
       <c r="I75" s="18"/>
       <c r="J75" s="18"/>
       <c r="K75" s="18"/>
-      <c r="L75" s="77"/>
+      <c r="L75" s="18"/>
       <c r="M75" s="18"/>
       <c r="N75" s="19"/>
       <c r="O75" s="19"/>
       <c r="P75" s="19"/>
       <c r="Q75" s="19"/>
-      <c r="R75" s="19"/>
+      <c r="R75" s="134"/>
       <c r="S75" s="20"/>
       <c r="T75" s="20"/>
       <c r="U75" s="20"/>
       <c r="V75" s="20"/>
-      <c r="W75" s="64"/>
+      <c r="W75" s="46"/>
       <c r="X75" s="33"/>
     </row>
     <row r="76" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="53"/>
-      <c r="B76" s="60"/>
-      <c r="C76" s="61"/>
-      <c r="D76" s="97"/>
-      <c r="E76" s="78"/>
-      <c r="F76" s="78"/>
-      <c r="G76" s="78"/>
-      <c r="H76" s="78"/>
-      <c r="I76" s="79"/>
-      <c r="J76" s="79"/>
-      <c r="K76" s="79"/>
-      <c r="L76" s="79"/>
-      <c r="M76" s="79"/>
-      <c r="N76" s="80"/>
-      <c r="O76" s="80"/>
-      <c r="P76" s="80"/>
-      <c r="Q76" s="80"/>
-      <c r="R76" s="80"/>
-      <c r="S76" s="81"/>
-      <c r="T76" s="81"/>
-      <c r="U76" s="81"/>
-      <c r="V76" s="81"/>
-      <c r="W76" s="64"/>
+      <c r="A76" s="87"/>
+      <c r="B76" s="98"/>
+      <c r="C76" s="99"/>
+      <c r="D76" s="63"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="53"/>
+      <c r="G76" s="53"/>
+      <c r="H76" s="53"/>
+      <c r="I76" s="52"/>
+      <c r="J76" s="52"/>
+      <c r="K76" s="52"/>
+      <c r="L76" s="52"/>
+      <c r="M76" s="52"/>
+      <c r="N76" s="55"/>
+      <c r="O76" s="55"/>
+      <c r="P76" s="55"/>
+      <c r="Q76" s="55"/>
+      <c r="R76" s="55"/>
+      <c r="S76" s="56"/>
+      <c r="T76" s="56"/>
+      <c r="U76" s="56"/>
+      <c r="V76" s="56"/>
+      <c r="W76" s="46"/>
       <c r="X76" s="33"/>
     </row>
     <row r="77" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="51">
+      <c r="A77" s="86">
         <f t="shared" ref="A77:A87" si="6">A75+1</f>
         <v>35</v>
       </c>
-      <c r="B77" s="60" t="s">
-        <v>64</v>
-      </c>
-      <c r="C77" s="61"/>
-      <c r="D77" s="57"/>
+      <c r="B77" s="98" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="99"/>
+      <c r="D77" s="43"/>
       <c r="E77" s="17"/>
       <c r="F77" s="17"/>
       <c r="G77" s="17"/>
@@ -4116,113 +4130,113 @@
       <c r="I77" s="18"/>
       <c r="J77" s="18"/>
       <c r="K77" s="18"/>
-      <c r="L77" s="77"/>
+      <c r="L77" s="18"/>
       <c r="M77" s="18"/>
       <c r="N77" s="19"/>
       <c r="O77" s="19"/>
       <c r="P77" s="19"/>
       <c r="Q77" s="19"/>
       <c r="R77" s="19"/>
-      <c r="S77" s="20"/>
+      <c r="S77" s="134"/>
       <c r="T77" s="20"/>
       <c r="U77" s="20"/>
       <c r="V77" s="20"/>
-      <c r="W77" s="64"/>
+      <c r="W77" s="46"/>
       <c r="X77" s="33"/>
     </row>
     <row r="78" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="53"/>
-      <c r="B78" s="98"/>
-      <c r="C78" s="99"/>
-      <c r="D78" s="97"/>
-      <c r="E78" s="78"/>
-      <c r="F78" s="78"/>
-      <c r="G78" s="78"/>
-      <c r="H78" s="78"/>
-      <c r="I78" s="79"/>
-      <c r="J78" s="79"/>
-      <c r="K78" s="79"/>
-      <c r="L78" s="79"/>
-      <c r="M78" s="79"/>
-      <c r="N78" s="80"/>
-      <c r="O78" s="80"/>
-      <c r="P78" s="80"/>
-      <c r="Q78" s="80"/>
-      <c r="R78" s="80"/>
-      <c r="S78" s="81"/>
-      <c r="T78" s="81"/>
-      <c r="U78" s="81"/>
-      <c r="V78" s="81"/>
-      <c r="W78" s="64"/>
+      <c r="A78" s="87"/>
+      <c r="B78" s="114"/>
+      <c r="C78" s="115"/>
+      <c r="D78" s="63"/>
+      <c r="E78" s="53"/>
+      <c r="F78" s="53"/>
+      <c r="G78" s="53"/>
+      <c r="H78" s="53"/>
+      <c r="I78" s="52"/>
+      <c r="J78" s="52"/>
+      <c r="K78" s="52"/>
+      <c r="L78" s="52"/>
+      <c r="M78" s="52"/>
+      <c r="N78" s="55"/>
+      <c r="O78" s="55"/>
+      <c r="P78" s="55"/>
+      <c r="Q78" s="55"/>
+      <c r="R78" s="55"/>
+      <c r="S78" s="56"/>
+      <c r="T78" s="56"/>
+      <c r="U78" s="56"/>
+      <c r="V78" s="56"/>
+      <c r="W78" s="46"/>
       <c r="X78" s="33"/>
     </row>
     <row r="79" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="51">
+      <c r="A79" s="86">
         <f t="shared" si="6"/>
         <v>36</v>
       </c>
-      <c r="B79" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="C79" s="83"/>
-      <c r="D79" s="123"/>
-      <c r="E79" s="124"/>
-      <c r="F79" s="124"/>
-      <c r="G79" s="124"/>
-      <c r="H79" s="124"/>
-      <c r="I79" s="95"/>
-      <c r="J79" s="95"/>
-      <c r="K79" s="95"/>
-      <c r="L79" s="95"/>
-      <c r="M79" s="77"/>
-      <c r="N79" s="125"/>
-      <c r="O79" s="125"/>
-      <c r="P79" s="125"/>
-      <c r="Q79" s="125"/>
-      <c r="R79" s="125"/>
-      <c r="S79" s="126"/>
-      <c r="T79" s="126"/>
-      <c r="U79" s="126"/>
-      <c r="V79" s="126"/>
-      <c r="W79" s="64"/>
+      <c r="B79" s="91" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" s="92"/>
+      <c r="D79" s="68"/>
+      <c r="E79" s="57"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="57"/>
+      <c r="H79" s="57"/>
+      <c r="I79" s="58"/>
+      <c r="J79" s="58"/>
+      <c r="K79" s="58"/>
+      <c r="L79" s="58"/>
+      <c r="M79" s="58"/>
+      <c r="N79" s="59"/>
+      <c r="O79" s="59"/>
+      <c r="P79" s="59"/>
+      <c r="Q79" s="59"/>
+      <c r="R79" s="59"/>
+      <c r="S79" s="61"/>
+      <c r="T79" s="135"/>
+      <c r="U79" s="61"/>
+      <c r="V79" s="61"/>
+      <c r="W79" s="46"/>
       <c r="X79" s="33"/>
     </row>
     <row r="80" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="53"/>
-      <c r="B80" s="84"/>
-      <c r="C80" s="85"/>
-      <c r="D80" s="123"/>
-      <c r="E80" s="124"/>
-      <c r="F80" s="124"/>
-      <c r="G80" s="124"/>
-      <c r="H80" s="124"/>
-      <c r="I80" s="95"/>
-      <c r="J80" s="95"/>
-      <c r="K80" s="95"/>
-      <c r="L80" s="95"/>
-      <c r="M80" s="79"/>
-      <c r="N80" s="125"/>
-      <c r="O80" s="125"/>
-      <c r="P80" s="125"/>
-      <c r="Q80" s="125"/>
-      <c r="R80" s="125"/>
-      <c r="S80" s="126"/>
-      <c r="T80" s="126"/>
-      <c r="U80" s="126"/>
-      <c r="V80" s="126"/>
-      <c r="W80" s="64"/>
+      <c r="A80" s="87"/>
+      <c r="B80" s="93"/>
+      <c r="C80" s="94"/>
+      <c r="D80" s="68"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="57"/>
+      <c r="H80" s="57"/>
+      <c r="I80" s="58"/>
+      <c r="J80" s="58"/>
+      <c r="K80" s="58"/>
+      <c r="L80" s="58"/>
+      <c r="M80" s="58"/>
+      <c r="N80" s="59"/>
+      <c r="O80" s="59"/>
+      <c r="P80" s="59"/>
+      <c r="Q80" s="59"/>
+      <c r="R80" s="59"/>
+      <c r="S80" s="61"/>
+      <c r="T80" s="61"/>
+      <c r="U80" s="61"/>
+      <c r="V80" s="61"/>
+      <c r="W80" s="46"/>
       <c r="X80" s="33"/>
     </row>
     <row r="81" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="51">
+      <c r="A81" s="86">
         <f t="shared" si="6"/>
         <v>37</v>
       </c>
-      <c r="B81" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C81" s="61"/>
-      <c r="D81" s="57"/>
+      <c r="B81" s="98" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" s="99"/>
+      <c r="D81" s="43"/>
       <c r="E81" s="17"/>
       <c r="F81" s="17"/>
       <c r="G81" s="17"/>
@@ -4232,54 +4246,54 @@
       <c r="K81" s="18"/>
       <c r="L81" s="18"/>
       <c r="M81" s="18"/>
-      <c r="N81" s="77"/>
+      <c r="N81" s="19"/>
       <c r="O81" s="19"/>
       <c r="P81" s="19"/>
       <c r="Q81" s="19"/>
       <c r="R81" s="19"/>
       <c r="S81" s="20"/>
-      <c r="T81" s="20"/>
+      <c r="T81" s="134"/>
       <c r="U81" s="20"/>
       <c r="V81" s="20"/>
-      <c r="W81" s="64"/>
+      <c r="W81" s="46"/>
       <c r="X81" s="33"/>
     </row>
     <row r="82" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="53"/>
-      <c r="B82" s="60"/>
-      <c r="C82" s="61"/>
-      <c r="D82" s="97"/>
-      <c r="E82" s="78"/>
-      <c r="F82" s="78"/>
-      <c r="G82" s="78"/>
-      <c r="H82" s="78"/>
-      <c r="I82" s="79"/>
-      <c r="J82" s="79"/>
-      <c r="K82" s="79"/>
-      <c r="L82" s="79"/>
-      <c r="M82" s="79"/>
-      <c r="N82" s="80"/>
-      <c r="O82" s="80"/>
-      <c r="P82" s="80"/>
-      <c r="Q82" s="80"/>
-      <c r="R82" s="80"/>
-      <c r="S82" s="81"/>
-      <c r="T82" s="81"/>
-      <c r="U82" s="81"/>
-      <c r="V82" s="81"/>
-      <c r="W82" s="64"/>
+      <c r="A82" s="87"/>
+      <c r="B82" s="98"/>
+      <c r="C82" s="99"/>
+      <c r="D82" s="63"/>
+      <c r="E82" s="53"/>
+      <c r="F82" s="53"/>
+      <c r="G82" s="53"/>
+      <c r="H82" s="53"/>
+      <c r="I82" s="52"/>
+      <c r="J82" s="52"/>
+      <c r="K82" s="52"/>
+      <c r="L82" s="52"/>
+      <c r="M82" s="52"/>
+      <c r="N82" s="55"/>
+      <c r="O82" s="55"/>
+      <c r="P82" s="55"/>
+      <c r="Q82" s="55"/>
+      <c r="R82" s="55"/>
+      <c r="S82" s="56"/>
+      <c r="T82" s="56"/>
+      <c r="U82" s="56"/>
+      <c r="V82" s="56"/>
+      <c r="W82" s="46"/>
       <c r="X82" s="33"/>
     </row>
     <row r="83" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="51">
+      <c r="A83" s="86">
         <f t="shared" si="6"/>
         <v>38</v>
       </c>
-      <c r="B83" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="C83" s="61"/>
-      <c r="D83" s="57"/>
+      <c r="B83" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="99"/>
+      <c r="D83" s="43"/>
       <c r="E83" s="17"/>
       <c r="F83" s="17"/>
       <c r="G83" s="17"/>
@@ -4290,53 +4304,53 @@
       <c r="L83" s="18"/>
       <c r="M83" s="18"/>
       <c r="N83" s="19"/>
-      <c r="O83" s="77"/>
+      <c r="O83" s="19"/>
       <c r="P83" s="19"/>
       <c r="Q83" s="19"/>
       <c r="R83" s="19"/>
       <c r="S83" s="20"/>
       <c r="T83" s="20"/>
-      <c r="U83" s="20"/>
+      <c r="U83" s="134"/>
       <c r="V83" s="20"/>
-      <c r="W83" s="64"/>
+      <c r="W83" s="46"/>
       <c r="X83" s="33"/>
     </row>
     <row r="84" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="53"/>
-      <c r="B84" s="60"/>
-      <c r="C84" s="61"/>
-      <c r="D84" s="97"/>
-      <c r="E84" s="78"/>
-      <c r="F84" s="78"/>
-      <c r="G84" s="78"/>
-      <c r="H84" s="78"/>
-      <c r="I84" s="79"/>
-      <c r="J84" s="79"/>
-      <c r="K84" s="79"/>
-      <c r="L84" s="79"/>
-      <c r="M84" s="79"/>
-      <c r="N84" s="80"/>
-      <c r="O84" s="80"/>
-      <c r="P84" s="80"/>
-      <c r="Q84" s="80"/>
-      <c r="R84" s="80"/>
-      <c r="S84" s="81"/>
-      <c r="T84" s="81"/>
-      <c r="U84" s="81"/>
-      <c r="V84" s="81"/>
-      <c r="W84" s="64"/>
+      <c r="A84" s="87"/>
+      <c r="B84" s="98"/>
+      <c r="C84" s="99"/>
+      <c r="D84" s="63"/>
+      <c r="E84" s="53"/>
+      <c r="F84" s="53"/>
+      <c r="G84" s="53"/>
+      <c r="H84" s="53"/>
+      <c r="I84" s="52"/>
+      <c r="J84" s="52"/>
+      <c r="K84" s="52"/>
+      <c r="L84" s="52"/>
+      <c r="M84" s="52"/>
+      <c r="N84" s="55"/>
+      <c r="O84" s="55"/>
+      <c r="P84" s="55"/>
+      <c r="Q84" s="55"/>
+      <c r="R84" s="55"/>
+      <c r="S84" s="56"/>
+      <c r="T84" s="56"/>
+      <c r="U84" s="56"/>
+      <c r="V84" s="56"/>
+      <c r="W84" s="46"/>
       <c r="X84" s="33"/>
     </row>
     <row r="85" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="51">
+      <c r="A85" s="86">
         <f t="shared" si="6"/>
         <v>39</v>
       </c>
-      <c r="B85" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="C85" s="61"/>
-      <c r="D85" s="57"/>
+      <c r="B85" s="98" t="s">
+        <v>31</v>
+      </c>
+      <c r="C85" s="99"/>
+      <c r="D85" s="43"/>
       <c r="E85" s="17"/>
       <c r="F85" s="17"/>
       <c r="G85" s="17"/>
@@ -4355,45 +4369,45 @@
       <c r="T85" s="20"/>
       <c r="U85" s="20"/>
       <c r="V85" s="20"/>
-      <c r="W85" s="64"/>
+      <c r="W85" s="46"/>
       <c r="X85" s="33"/>
     </row>
     <row r="86" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="53"/>
-      <c r="B86" s="60"/>
-      <c r="C86" s="61"/>
-      <c r="D86" s="97"/>
-      <c r="E86" s="78"/>
-      <c r="F86" s="78"/>
-      <c r="G86" s="78"/>
-      <c r="H86" s="78"/>
-      <c r="I86" s="79"/>
-      <c r="J86" s="79"/>
-      <c r="K86" s="79"/>
-      <c r="L86" s="79"/>
-      <c r="M86" s="79"/>
-      <c r="N86" s="80"/>
-      <c r="O86" s="80"/>
-      <c r="P86" s="80"/>
-      <c r="Q86" s="80"/>
-      <c r="R86" s="80"/>
-      <c r="S86" s="81"/>
-      <c r="T86" s="81"/>
-      <c r="U86" s="81"/>
-      <c r="V86" s="81"/>
-      <c r="W86" s="64"/>
+      <c r="A86" s="87"/>
+      <c r="B86" s="98"/>
+      <c r="C86" s="99"/>
+      <c r="D86" s="63"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="53"/>
+      <c r="G86" s="53"/>
+      <c r="H86" s="53"/>
+      <c r="I86" s="52"/>
+      <c r="J86" s="52"/>
+      <c r="K86" s="52"/>
+      <c r="L86" s="52"/>
+      <c r="M86" s="52"/>
+      <c r="N86" s="55"/>
+      <c r="O86" s="55"/>
+      <c r="P86" s="55"/>
+      <c r="Q86" s="55"/>
+      <c r="R86" s="55"/>
+      <c r="S86" s="56"/>
+      <c r="T86" s="56"/>
+      <c r="U86" s="56"/>
+      <c r="V86" s="56"/>
+      <c r="W86" s="46"/>
       <c r="X86" s="33"/>
     </row>
     <row r="87" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="51">
+      <c r="A87" s="86">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="B87" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="C87" s="61"/>
-      <c r="D87" s="57"/>
+      <c r="B87" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="C87" s="99"/>
+      <c r="D87" s="43"/>
       <c r="E87" s="17"/>
       <c r="F87" s="17"/>
       <c r="G87" s="17"/>
@@ -4410,45 +4424,45 @@
       <c r="R87" s="19"/>
       <c r="S87" s="20"/>
       <c r="T87" s="20"/>
-      <c r="U87" s="20"/>
-      <c r="V87" s="20"/>
-      <c r="W87" s="64"/>
+      <c r="U87" s="54"/>
+      <c r="V87" s="54"/>
+      <c r="W87" s="46"/>
       <c r="X87" s="33"/>
     </row>
     <row r="88" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="53"/>
-      <c r="B88" s="60"/>
-      <c r="C88" s="61"/>
-      <c r="D88" s="97"/>
-      <c r="E88" s="78"/>
-      <c r="F88" s="78"/>
-      <c r="G88" s="78"/>
-      <c r="H88" s="78"/>
-      <c r="I88" s="79"/>
-      <c r="J88" s="79"/>
-      <c r="K88" s="79"/>
-      <c r="L88" s="79"/>
-      <c r="M88" s="79"/>
-      <c r="N88" s="80"/>
-      <c r="O88" s="80"/>
-      <c r="P88" s="80"/>
-      <c r="Q88" s="80"/>
-      <c r="R88" s="80"/>
-      <c r="S88" s="81"/>
-      <c r="T88" s="81"/>
-      <c r="U88" s="81"/>
-      <c r="V88" s="81"/>
-      <c r="W88" s="64"/>
+      <c r="A88" s="87"/>
+      <c r="B88" s="98"/>
+      <c r="C88" s="99"/>
+      <c r="D88" s="63"/>
+      <c r="E88" s="53"/>
+      <c r="F88" s="53"/>
+      <c r="G88" s="53"/>
+      <c r="H88" s="53"/>
+      <c r="I88" s="52"/>
+      <c r="J88" s="52"/>
+      <c r="K88" s="52"/>
+      <c r="L88" s="52"/>
+      <c r="M88" s="52"/>
+      <c r="N88" s="55"/>
+      <c r="O88" s="55"/>
+      <c r="P88" s="55"/>
+      <c r="Q88" s="55"/>
+      <c r="R88" s="55"/>
+      <c r="S88" s="56"/>
+      <c r="T88" s="56"/>
+      <c r="U88" s="56"/>
+      <c r="V88" s="56"/>
+      <c r="W88" s="46"/>
       <c r="X88" s="33"/>
     </row>
     <row r="89" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="51">
+      <c r="A89" s="86">
         <f t="shared" ref="A89:A99" si="7">A87+1</f>
         <v>41</v>
       </c>
-      <c r="B89" s="114"/>
-      <c r="C89" s="115"/>
-      <c r="D89" s="57"/>
+      <c r="B89" s="96"/>
+      <c r="C89" s="97"/>
+      <c r="D89" s="43"/>
       <c r="E89" s="17"/>
       <c r="F89" s="17"/>
       <c r="G89" s="17"/>
@@ -4467,43 +4481,43 @@
       <c r="T89" s="20"/>
       <c r="U89" s="20"/>
       <c r="V89" s="20"/>
-      <c r="W89" s="64"/>
+      <c r="W89" s="46"/>
       <c r="X89" s="33"/>
     </row>
     <row r="90" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="53"/>
-      <c r="B90" s="114"/>
-      <c r="C90" s="115"/>
-      <c r="D90" s="97"/>
-      <c r="E90" s="78"/>
-      <c r="F90" s="78"/>
-      <c r="G90" s="78"/>
-      <c r="H90" s="78"/>
-      <c r="I90" s="79"/>
-      <c r="J90" s="79"/>
-      <c r="K90" s="79"/>
-      <c r="L90" s="79"/>
-      <c r="M90" s="79"/>
-      <c r="N90" s="80"/>
-      <c r="O90" s="80"/>
-      <c r="P90" s="80"/>
-      <c r="Q90" s="80"/>
-      <c r="R90" s="80"/>
-      <c r="S90" s="81"/>
-      <c r="T90" s="81"/>
-      <c r="U90" s="81"/>
-      <c r="V90" s="81"/>
-      <c r="W90" s="64"/>
+      <c r="A90" s="87"/>
+      <c r="B90" s="96"/>
+      <c r="C90" s="97"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="53"/>
+      <c r="F90" s="53"/>
+      <c r="G90" s="53"/>
+      <c r="H90" s="53"/>
+      <c r="I90" s="52"/>
+      <c r="J90" s="52"/>
+      <c r="K90" s="52"/>
+      <c r="L90" s="52"/>
+      <c r="M90" s="52"/>
+      <c r="N90" s="55"/>
+      <c r="O90" s="55"/>
+      <c r="P90" s="55"/>
+      <c r="Q90" s="55"/>
+      <c r="R90" s="55"/>
+      <c r="S90" s="56"/>
+      <c r="T90" s="56"/>
+      <c r="U90" s="56"/>
+      <c r="V90" s="56"/>
+      <c r="W90" s="46"/>
       <c r="X90" s="33"/>
     </row>
     <row r="91" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="51">
+      <c r="A91" s="86">
         <f t="shared" si="7"/>
         <v>42</v>
       </c>
-      <c r="B91" s="114"/>
-      <c r="C91" s="115"/>
-      <c r="D91" s="57"/>
+      <c r="B91" s="96"/>
+      <c r="C91" s="97"/>
+      <c r="D91" s="43"/>
       <c r="E91" s="17"/>
       <c r="F91" s="17"/>
       <c r="G91" s="17"/>
@@ -4522,43 +4536,43 @@
       <c r="T91" s="20"/>
       <c r="U91" s="20"/>
       <c r="V91" s="20"/>
-      <c r="W91" s="64"/>
+      <c r="W91" s="46"/>
       <c r="X91" s="33"/>
     </row>
     <row r="92" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="53"/>
-      <c r="B92" s="114"/>
-      <c r="C92" s="115"/>
-      <c r="D92" s="97"/>
-      <c r="E92" s="78"/>
-      <c r="F92" s="78"/>
-      <c r="G92" s="78"/>
-      <c r="H92" s="78"/>
-      <c r="I92" s="79"/>
-      <c r="J92" s="79"/>
-      <c r="K92" s="79"/>
-      <c r="L92" s="79"/>
-      <c r="M92" s="79"/>
-      <c r="N92" s="80"/>
-      <c r="O92" s="80"/>
-      <c r="P92" s="80"/>
-      <c r="Q92" s="80"/>
-      <c r="R92" s="80"/>
-      <c r="S92" s="81"/>
-      <c r="T92" s="81"/>
-      <c r="U92" s="81"/>
-      <c r="V92" s="81"/>
-      <c r="W92" s="64"/>
+      <c r="A92" s="87"/>
+      <c r="B92" s="96"/>
+      <c r="C92" s="97"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="53"/>
+      <c r="F92" s="53"/>
+      <c r="G92" s="53"/>
+      <c r="H92" s="53"/>
+      <c r="I92" s="52"/>
+      <c r="J92" s="52"/>
+      <c r="K92" s="52"/>
+      <c r="L92" s="52"/>
+      <c r="M92" s="52"/>
+      <c r="N92" s="55"/>
+      <c r="O92" s="55"/>
+      <c r="P92" s="55"/>
+      <c r="Q92" s="55"/>
+      <c r="R92" s="55"/>
+      <c r="S92" s="56"/>
+      <c r="T92" s="56"/>
+      <c r="U92" s="56"/>
+      <c r="V92" s="56"/>
+      <c r="W92" s="46"/>
       <c r="X92" s="33"/>
     </row>
     <row r="93" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="51">
+      <c r="A93" s="86">
         <f t="shared" si="7"/>
         <v>43</v>
       </c>
-      <c r="B93" s="60"/>
-      <c r="C93" s="61"/>
-      <c r="D93" s="57"/>
+      <c r="B93" s="98"/>
+      <c r="C93" s="99"/>
+      <c r="D93" s="43"/>
       <c r="E93" s="17"/>
       <c r="F93" s="17"/>
       <c r="G93" s="17"/>
@@ -4577,43 +4591,43 @@
       <c r="T93" s="20"/>
       <c r="U93" s="20"/>
       <c r="V93" s="20"/>
-      <c r="W93" s="64"/>
+      <c r="W93" s="46"/>
       <c r="X93" s="33"/>
     </row>
     <row r="94" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="53"/>
-      <c r="B94" s="60"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="97"/>
-      <c r="E94" s="78"/>
-      <c r="F94" s="78"/>
-      <c r="G94" s="78"/>
-      <c r="H94" s="78"/>
-      <c r="I94" s="79"/>
-      <c r="J94" s="79"/>
-      <c r="K94" s="79"/>
-      <c r="L94" s="79"/>
-      <c r="M94" s="79"/>
-      <c r="N94" s="80"/>
-      <c r="O94" s="80"/>
-      <c r="P94" s="80"/>
-      <c r="Q94" s="80"/>
-      <c r="R94" s="80"/>
-      <c r="S94" s="81"/>
-      <c r="T94" s="81"/>
-      <c r="U94" s="81"/>
-      <c r="V94" s="81"/>
-      <c r="W94" s="64"/>
+      <c r="A94" s="87"/>
+      <c r="B94" s="98"/>
+      <c r="C94" s="99"/>
+      <c r="D94" s="63"/>
+      <c r="E94" s="53"/>
+      <c r="F94" s="53"/>
+      <c r="G94" s="53"/>
+      <c r="H94" s="53"/>
+      <c r="I94" s="52"/>
+      <c r="J94" s="52"/>
+      <c r="K94" s="52"/>
+      <c r="L94" s="52"/>
+      <c r="M94" s="52"/>
+      <c r="N94" s="55"/>
+      <c r="O94" s="55"/>
+      <c r="P94" s="55"/>
+      <c r="Q94" s="55"/>
+      <c r="R94" s="55"/>
+      <c r="S94" s="56"/>
+      <c r="T94" s="56"/>
+      <c r="U94" s="56"/>
+      <c r="V94" s="56"/>
+      <c r="W94" s="46"/>
       <c r="X94" s="33"/>
     </row>
     <row r="95" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="51">
+      <c r="A95" s="86">
         <f t="shared" si="7"/>
         <v>44</v>
       </c>
-      <c r="B95" s="116"/>
-      <c r="C95" s="117"/>
-      <c r="D95" s="57"/>
+      <c r="B95" s="100"/>
+      <c r="C95" s="101"/>
+      <c r="D95" s="43"/>
       <c r="E95" s="17"/>
       <c r="F95" s="17"/>
       <c r="G95" s="17"/>
@@ -4632,43 +4646,43 @@
       <c r="T95" s="20"/>
       <c r="U95" s="20"/>
       <c r="V95" s="20"/>
-      <c r="W95" s="64"/>
+      <c r="W95" s="46"/>
       <c r="X95" s="33"/>
     </row>
     <row r="96" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="53"/>
-      <c r="B96" s="116"/>
-      <c r="C96" s="117"/>
-      <c r="D96" s="97"/>
-      <c r="E96" s="78"/>
-      <c r="F96" s="78"/>
-      <c r="G96" s="78"/>
-      <c r="H96" s="78"/>
-      <c r="I96" s="79"/>
-      <c r="J96" s="79"/>
-      <c r="K96" s="79"/>
-      <c r="L96" s="79"/>
-      <c r="M96" s="79"/>
-      <c r="N96" s="80"/>
-      <c r="O96" s="80"/>
-      <c r="P96" s="80"/>
-      <c r="Q96" s="80"/>
-      <c r="R96" s="80"/>
-      <c r="S96" s="81"/>
-      <c r="T96" s="81"/>
-      <c r="U96" s="81"/>
-      <c r="V96" s="81"/>
-      <c r="W96" s="64"/>
+      <c r="A96" s="87"/>
+      <c r="B96" s="100"/>
+      <c r="C96" s="101"/>
+      <c r="D96" s="63"/>
+      <c r="E96" s="53"/>
+      <c r="F96" s="53"/>
+      <c r="G96" s="53"/>
+      <c r="H96" s="53"/>
+      <c r="I96" s="52"/>
+      <c r="J96" s="52"/>
+      <c r="K96" s="52"/>
+      <c r="L96" s="52"/>
+      <c r="M96" s="52"/>
+      <c r="N96" s="55"/>
+      <c r="O96" s="55"/>
+      <c r="P96" s="55"/>
+      <c r="Q96" s="55"/>
+      <c r="R96" s="55"/>
+      <c r="S96" s="56"/>
+      <c r="T96" s="56"/>
+      <c r="U96" s="56"/>
+      <c r="V96" s="56"/>
+      <c r="W96" s="46"/>
       <c r="X96" s="33"/>
     </row>
     <row r="97" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="51">
+      <c r="A97" s="86">
         <f t="shared" si="7"/>
         <v>45</v>
       </c>
-      <c r="B97" s="114"/>
-      <c r="C97" s="115"/>
-      <c r="D97" s="57"/>
+      <c r="B97" s="96"/>
+      <c r="C97" s="97"/>
+      <c r="D97" s="43"/>
       <c r="E97" s="17"/>
       <c r="F97" s="17"/>
       <c r="G97" s="17"/>
@@ -4687,42 +4701,42 @@
       <c r="T97" s="20"/>
       <c r="U97" s="20"/>
       <c r="V97" s="20"/>
-      <c r="W97" s="64"/>
+      <c r="W97" s="46"/>
       <c r="X97" s="33"/>
     </row>
     <row r="98" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="53"/>
-      <c r="B98" s="114"/>
-      <c r="C98" s="115"/>
-      <c r="D98" s="97"/>
-      <c r="E98" s="78"/>
-      <c r="F98" s="78"/>
-      <c r="G98" s="78"/>
-      <c r="H98" s="78"/>
-      <c r="I98" s="79"/>
-      <c r="J98" s="79"/>
-      <c r="K98" s="79"/>
-      <c r="L98" s="79"/>
-      <c r="M98" s="79"/>
-      <c r="N98" s="80"/>
-      <c r="O98" s="80"/>
-      <c r="P98" s="80"/>
-      <c r="Q98" s="80"/>
-      <c r="R98" s="80"/>
-      <c r="S98" s="81"/>
-      <c r="T98" s="81"/>
-      <c r="U98" s="81"/>
-      <c r="V98" s="81"/>
-      <c r="W98" s="67"/>
+      <c r="A98" s="87"/>
+      <c r="B98" s="96"/>
+      <c r="C98" s="97"/>
+      <c r="D98" s="63"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="53"/>
+      <c r="G98" s="53"/>
+      <c r="H98" s="53"/>
+      <c r="I98" s="52"/>
+      <c r="J98" s="52"/>
+      <c r="K98" s="52"/>
+      <c r="L98" s="52"/>
+      <c r="M98" s="52"/>
+      <c r="N98" s="55"/>
+      <c r="O98" s="55"/>
+      <c r="P98" s="55"/>
+      <c r="Q98" s="55"/>
+      <c r="R98" s="55"/>
+      <c r="S98" s="56"/>
+      <c r="T98" s="56"/>
+      <c r="U98" s="56"/>
+      <c r="V98" s="56"/>
+      <c r="W98" s="49"/>
       <c r="X98" s="34"/>
     </row>
     <row r="99" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="51">
+      <c r="A99" s="86">
         <f t="shared" si="7"/>
         <v>46</v>
       </c>
-      <c r="B99" s="53"/>
-      <c r="C99" s="92"/>
+      <c r="B99" s="87"/>
+      <c r="C99" s="88"/>
       <c r="D99" s="15"/>
       <c r="E99" s="15"/>
       <c r="F99" s="1"/>
@@ -4743,17 +4757,17 @@
       <c r="U99" s="15"/>
       <c r="V99" s="15"/>
       <c r="W99" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X99" s="7"/>
     </row>
     <row r="100" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="53"/>
-      <c r="B100" s="93"/>
-      <c r="C100" s="94"/>
-      <c r="D100" s="107"/>
+      <c r="A100" s="87"/>
+      <c r="B100" s="89"/>
+      <c r="C100" s="90"/>
+      <c r="D100" s="69"/>
       <c r="E100" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="3"/>
@@ -4773,17 +4787,17 @@
       <c r="U100" s="15"/>
       <c r="V100" s="15"/>
       <c r="W100" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X100" s="8"/>
     </row>
     <row r="101" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="35"/>
       <c r="B101" s="37"/>
-      <c r="C101" s="65"/>
-      <c r="D101" s="127"/>
+      <c r="C101" s="47"/>
+      <c r="D101" s="80"/>
       <c r="E101" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
@@ -4809,9 +4823,9 @@
       <c r="A102" s="36"/>
       <c r="B102" s="36"/>
       <c r="C102" s="38"/>
-      <c r="D102" s="108"/>
+      <c r="D102" s="70"/>
       <c r="E102" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F102" s="15"/>
       <c r="G102" s="15"/>
@@ -4891,7 +4905,7 @@
       <c r="C105" s="24"/>
       <c r="D105" s="15"/>
       <c r="E105" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F105" s="15"/>
       <c r="G105" s="15"/>
@@ -4915,9 +4929,9 @@
     </row>
     <row r="106" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="15"/>
-      <c r="B106" s="118"/>
-      <c r="C106" s="119" t="s">
-        <v>22</v>
+      <c r="B106" s="75"/>
+      <c r="C106" s="76" t="s">
+        <v>21</v>
       </c>
       <c r="D106" s="15"/>
       <c r="E106" s="15"/>
@@ -4943,11 +4957,11 @@
     </row>
     <row r="107" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="15"/>
-      <c r="B107" s="101"/>
+      <c r="B107" s="65"/>
       <c r="C107" s="24"/>
       <c r="D107" s="15"/>
       <c r="E107" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F107" s="15"/>
       <c r="G107" s="15"/>
@@ -4971,33 +4985,33 @@
     </row>
     <row r="108" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="15"/>
-      <c r="B108" s="101"/>
+      <c r="B108" s="65"/>
       <c r="C108" s="24"/>
     </row>
     <row r="109" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="15"/>
-      <c r="B109" s="101"/>
+      <c r="B109" s="65"/>
       <c r="C109" s="24"/>
       <c r="E109" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="101"/>
+      <c r="B110" s="65"/>
       <c r="C110" s="24"/>
     </row>
     <row r="111" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="101"/>
-      <c r="C111" s="119" t="s">
-        <v>27</v>
+      <c r="B111" s="65"/>
+      <c r="C111" s="76" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="112" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="101"/>
+      <c r="B112" s="65"/>
       <c r="C112" s="24"/>
     </row>
     <row r="113" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="101"/>
+      <c r="B113" s="65"/>
       <c r="C113" s="24"/>
     </row>
     <row r="114" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5011,12 +5025,99 @@
     <row r="119" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="121" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="122" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C122" s="122"/>
+      <c r="C122" s="79"/>
     </row>
     <row r="123" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="124" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="111">
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="J68:J70"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="B32:C33"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B71:C72"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B75:C76"/>
+    <mergeCell ref="G4:R5"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="B46:C47"/>
+    <mergeCell ref="B48:C49"/>
+    <mergeCell ref="B50:C51"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="T68:T70"/>
+    <mergeCell ref="U68:U70"/>
+    <mergeCell ref="V68:V70"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="B40:C41"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B44:C45"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B52:C53"/>
+    <mergeCell ref="B54:C55"/>
+    <mergeCell ref="B56:C57"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="B60:C61"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="B64:C65"/>
+    <mergeCell ref="B66:C67"/>
+    <mergeCell ref="B73:C74"/>
+    <mergeCell ref="B68:C70"/>
+    <mergeCell ref="B87:C88"/>
+    <mergeCell ref="P68:P70"/>
+    <mergeCell ref="Q68:Q70"/>
+    <mergeCell ref="R68:R70"/>
+    <mergeCell ref="S68:S70"/>
+    <mergeCell ref="K68:K70"/>
+    <mergeCell ref="L68:L70"/>
+    <mergeCell ref="M68:M70"/>
+    <mergeCell ref="N68:N70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="H68:H70"/>
+    <mergeCell ref="I68:I70"/>
+    <mergeCell ref="B77:C78"/>
+    <mergeCell ref="D68:D70"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B99:C100"/>
@@ -5041,93 +5142,6 @@
     <mergeCell ref="B81:C82"/>
     <mergeCell ref="B83:C84"/>
     <mergeCell ref="B85:C86"/>
-    <mergeCell ref="B87:C88"/>
-    <mergeCell ref="O68:O70"/>
-    <mergeCell ref="P68:P70"/>
-    <mergeCell ref="Q68:Q70"/>
-    <mergeCell ref="R68:R70"/>
-    <mergeCell ref="S68:S70"/>
-    <mergeCell ref="K68:K70"/>
-    <mergeCell ref="L68:L70"/>
-    <mergeCell ref="M68:M70"/>
-    <mergeCell ref="N68:N70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="F68:F70"/>
-    <mergeCell ref="G68:G70"/>
-    <mergeCell ref="H68:H70"/>
-    <mergeCell ref="I68:I70"/>
-    <mergeCell ref="B52:C53"/>
-    <mergeCell ref="B54:C55"/>
-    <mergeCell ref="B56:C57"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="B60:C61"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="B64:C65"/>
-    <mergeCell ref="B66:C67"/>
-    <mergeCell ref="B73:C74"/>
-    <mergeCell ref="B77:C78"/>
-    <mergeCell ref="B68:C70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="T68:T70"/>
-    <mergeCell ref="U68:U70"/>
-    <mergeCell ref="V68:V70"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="B40:C41"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B44:C45"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="B46:C47"/>
-    <mergeCell ref="B48:C49"/>
-    <mergeCell ref="B50:C51"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="G4:R5"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="B32:C33"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B71:C72"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B75:C76"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -5144,14 +5158,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa56a77c-e65c-474c-a103-f5e192bb7a19">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="b9bdf651-246d-46a5-b6e2-05b72ee92a60" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5410,21 +5422,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa56a77c-e65c-474c-a103-f5e192bb7a19">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b9bdf651-246d-46a5-b6e2-05b72ee92a60" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91C011EA-11C9-4190-B994-E4384572B07C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1078420-64D2-42A2-96B9-547D7699446D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="aa56a77c-e65c-474c-a103-f5e192bb7a19"/>
-    <ds:schemaRef ds:uri="b9bdf651-246d-46a5-b6e2-05b72ee92a60"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5449,9 +5460,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1078420-64D2-42A2-96B9-547D7699446D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91C011EA-11C9-4190-B994-E4384572B07C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aa56a77c-e65c-474c-a103-f5e192bb7a19"/>
+    <ds:schemaRef ds:uri="b9bdf651-246d-46a5-b6e2-05b72ee92a60"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>